<commit_message>
Fix report 2 (HCA) autoscaling
</commit_message>
<xml_diff>
--- a/sprawozdanie1/distance_matrix.xlsx
+++ b/sprawozdanie1/distance_matrix.xlsx
@@ -533,91 +533,91 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1715402942088392</v>
+        <v>4.275319496401021</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1096679440594839</v>
+        <v>5.859271268402654</v>
       </c>
       <c r="E2" t="n">
-        <v>0.09396989250265395</v>
+        <v>2.965570259545592</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0761368726809649</v>
+        <v>2.96580115592548</v>
       </c>
       <c r="G2" t="n">
-        <v>0.1500929185360762</v>
+        <v>3.832217408651611</v>
       </c>
       <c r="H2" t="n">
-        <v>0.1676990804217875</v>
+        <v>3.327347127053255</v>
       </c>
       <c r="I2" t="n">
-        <v>0.1170792897661876</v>
+        <v>5.00327896930066</v>
       </c>
       <c r="J2" t="n">
-        <v>0.2731512824239208</v>
+        <v>8.178093993708188</v>
       </c>
       <c r="K2" t="n">
-        <v>0.1526425676485503</v>
+        <v>4.157587822854066</v>
       </c>
       <c r="L2" t="n">
-        <v>0.2206008644122393</v>
+        <v>5.412135499019779</v>
       </c>
       <c r="M2" t="n">
-        <v>0.2252101835970057</v>
+        <v>5.982288785562577</v>
       </c>
       <c r="N2" t="n">
-        <v>0.1398273506350843</v>
+        <v>6.649882146058538</v>
       </c>
       <c r="O2" t="n">
-        <v>0.2025138145825583</v>
+        <v>4.738182926070425</v>
       </c>
       <c r="P2" t="n">
-        <v>0.1004080704858452</v>
+        <v>3.561225118834551</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.08550039492222347</v>
+        <v>2.767369523368556</v>
       </c>
       <c r="R2" t="n">
-        <v>0.05933621753647254</v>
+        <v>2.598761112483388</v>
       </c>
       <c r="S2" t="n">
-        <v>0.08154452064721616</v>
+        <v>3.14790077987135</v>
       </c>
       <c r="T2" t="n">
-        <v>0.1695531917721534</v>
+        <v>4.634872707588587</v>
       </c>
       <c r="U2" t="n">
-        <v>0.09699225377234293</v>
+        <v>2.695516964504267</v>
       </c>
       <c r="V2" t="n">
-        <v>0.1101634197502209</v>
+        <v>4.31965444962708</v>
       </c>
       <c r="W2" t="n">
-        <v>0.1899452753901378</v>
+        <v>6.360367957504774</v>
       </c>
       <c r="X2" t="n">
-        <v>0.06581907329878174</v>
+        <v>1.637300194075228</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.2459834353226894</v>
+        <v>5.712427156349889</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.106795820175408</v>
+        <v>3.988916103650405</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.05554315646779839</v>
+        <v>2.21124761847412</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.1357325824031616</v>
+        <v>3.735023094091162</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.05226604243798294</v>
+        <v>2.013613563952808</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.04506818649620872</v>
+        <v>1.701564685390132</v>
       </c>
       <c r="AE2" t="n">
-        <v>0.2780711605469107</v>
+        <v>6.091820854177365</v>
       </c>
     </row>
     <row r="3">
@@ -625,94 +625,94 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.1715402942088392</v>
+        <v>4.275319496401021</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1275957675708383</v>
+        <v>3.16857258322564</v>
       </c>
       <c r="E3" t="n">
-        <v>0.08704228259505489</v>
+        <v>2.254434998016158</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1063571409170463</v>
+        <v>1.86463661192302</v>
       </c>
       <c r="G3" t="n">
-        <v>0.02583556033628069</v>
+        <v>1.169465854431525</v>
       </c>
       <c r="H3" t="n">
-        <v>0.02890680673827246</v>
+        <v>1.906998640956483</v>
       </c>
       <c r="I3" t="n">
-        <v>0.1108070403331864</v>
+        <v>2.774527167876043</v>
       </c>
       <c r="J3" t="n">
-        <v>0.103025345443509</v>
+        <v>3.978835286111829</v>
       </c>
       <c r="K3" t="n">
-        <v>0.03219421679668644</v>
+        <v>1.49285728833284</v>
       </c>
       <c r="L3" t="n">
-        <v>0.0517059847305083</v>
+        <v>1.428777426463639</v>
       </c>
       <c r="M3" t="n">
-        <v>0.05669802497754553</v>
+        <v>2.037703753661898</v>
       </c>
       <c r="N3" t="n">
-        <v>0.1626016982039385</v>
+        <v>3.920272848881794</v>
       </c>
       <c r="O3" t="n">
-        <v>0.03688028570382887</v>
+        <v>0.8161055600022139</v>
       </c>
       <c r="P3" t="n">
-        <v>0.09663050145433673</v>
+        <v>1.719034027001325</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.2056706577428302</v>
+        <v>3.675524341203782</v>
       </c>
       <c r="R3" t="n">
-        <v>0.1580751883247034</v>
+        <v>3.122229747150397</v>
       </c>
       <c r="S3" t="n">
-        <v>0.1590478083411667</v>
+        <v>3.117626289337508</v>
       </c>
       <c r="T3" t="n">
-        <v>0.03447710624140341</v>
+        <v>1.711905118640308</v>
       </c>
       <c r="U3" t="n">
-        <v>0.2164221395242461</v>
+        <v>3.755023586331237</v>
       </c>
       <c r="V3" t="n">
-        <v>0.1060777649125607</v>
+        <v>2.004260683280279</v>
       </c>
       <c r="W3" t="n">
-        <v>0.04223690453943452</v>
+        <v>2.349546033947658</v>
       </c>
       <c r="X3" t="n">
-        <v>0.111020922625073</v>
+        <v>3.341477486609099</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.08213880702039783</v>
+        <v>2.240793072687274</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.09982106388597427</v>
+        <v>2.227514640590237</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.1499077543743874</v>
+        <v>2.899974565947792</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.03824743763421085</v>
+        <v>1.18661481226105</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.1633172698707854</v>
+        <v>3.884251233197155</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.157114999240016</v>
+        <v>3.252804243130963</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.1127749837285775</v>
+        <v>2.419703202153505</v>
       </c>
     </row>
     <row r="4">
@@ -720,94 +720,94 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.1096679440594839</v>
+        <v>5.859271268402654</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1275957675708383</v>
+        <v>3.16857258322564</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.06926569207061699</v>
+        <v>4.201558471454018</v>
       </c>
       <c r="F4" t="n">
-        <v>0.05236603245060583</v>
+        <v>3.09855209177868</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1094443411160679</v>
+        <v>3.793136514983324</v>
       </c>
       <c r="H4" t="n">
-        <v>0.1386122169166829</v>
+        <v>4.24295364256685</v>
       </c>
       <c r="I4" t="n">
-        <v>0.04247425814485747</v>
+        <v>3.324329898372299</v>
       </c>
       <c r="J4" t="n">
-        <v>0.2225502853898075</v>
+        <v>4.884540589621968</v>
       </c>
       <c r="K4" t="n">
-        <v>0.103272425056116</v>
+        <v>3.780850335825918</v>
       </c>
       <c r="L4" t="n">
-        <v>0.1751484668589876</v>
+        <v>3.358405354585214</v>
       </c>
       <c r="M4" t="n">
-        <v>0.1792538855410932</v>
+        <v>3.291429531873295</v>
       </c>
       <c r="N4" t="n">
-        <v>0.04569867082713736</v>
+        <v>1.717103940274897</v>
       </c>
       <c r="O4" t="n">
-        <v>0.1643767192334777</v>
+        <v>3.760408479238031</v>
       </c>
       <c r="P4" t="n">
-        <v>0.03672827384948462</v>
+        <v>2.502264969245576</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.08989481022093464</v>
+        <v>3.641278611538448</v>
       </c>
       <c r="R4" t="n">
-        <v>0.05880516976923385</v>
+        <v>3.503876573838752</v>
       </c>
       <c r="S4" t="n">
-        <v>0.05333489253446617</v>
+        <v>4.021480431751958</v>
       </c>
       <c r="T4" t="n">
-        <v>0.1090201844341099</v>
+        <v>2.546009891248666</v>
       </c>
       <c r="U4" t="n">
-        <v>0.09906558595463066</v>
+        <v>4.056942536646842</v>
       </c>
       <c r="V4" t="n">
-        <v>0.0223858684056301</v>
+        <v>1.72120595170779</v>
       </c>
       <c r="W4" t="n">
-        <v>0.1204142087585774</v>
+        <v>2.486013600115259</v>
       </c>
       <c r="X4" t="n">
-        <v>0.07563297178059294</v>
+        <v>4.808886555729749</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.2063163315849977</v>
+        <v>4.054397494436631</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.03299209730288376</v>
+        <v>2.112175570209989</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.05621275750246625</v>
+        <v>3.691168026956802</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.09829304000566533</v>
+        <v>2.932309990850223</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.07127289197002133</v>
+        <v>4.620856073568758</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.06827564202121632</v>
+        <v>4.237882719954387</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.238154108792853</v>
+        <v>5.034943134914101</v>
       </c>
     </row>
     <row r="5">
@@ -815,94 +815,94 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.09396989250265395</v>
+        <v>2.965570259545592</v>
       </c>
       <c r="C5" t="n">
-        <v>0.08704228259505489</v>
+        <v>2.254434998016158</v>
       </c>
       <c r="D5" t="n">
-        <v>0.06926569207061699</v>
+        <v>4.201558471454018</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.02768258139341985</v>
+        <v>1.445842074678641</v>
       </c>
       <c r="G5" t="n">
-        <v>0.06248001822044158</v>
+        <v>1.283212431979839</v>
       </c>
       <c r="H5" t="n">
-        <v>0.09484454532190006</v>
+        <v>2.896939806723232</v>
       </c>
       <c r="I5" t="n">
-        <v>0.04967780776808293</v>
+        <v>2.229845541437901</v>
       </c>
       <c r="J5" t="n">
-        <v>0.1869129579960482</v>
+        <v>5.615539234913368</v>
       </c>
       <c r="K5" t="n">
-        <v>0.06144914692949361</v>
+        <v>1.358322179448296</v>
       </c>
       <c r="L5" t="n">
-        <v>0.1386683020797322</v>
+        <v>3.679437396973325</v>
       </c>
       <c r="M5" t="n">
-        <v>0.1436865963437164</v>
+        <v>4.283590739917385</v>
       </c>
       <c r="N5" t="n">
-        <v>0.1066659509039129</v>
+        <v>4.504453589626598</v>
       </c>
       <c r="O5" t="n">
-        <v>0.1211374580608665</v>
+        <v>2.731175742241764</v>
       </c>
       <c r="P5" t="n">
-        <v>0.03530546654983772</v>
+        <v>1.88676867875883</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.1274004179708874</v>
+        <v>3.037540912504872</v>
       </c>
       <c r="R5" t="n">
-        <v>0.08245061718406671</v>
+        <v>2.848295112824452</v>
       </c>
       <c r="S5" t="n">
-        <v>0.07760526225878886</v>
+        <v>1.332068341822178</v>
       </c>
       <c r="T5" t="n">
-        <v>0.08789601675861024</v>
+        <v>3.436736765950698</v>
       </c>
       <c r="U5" t="n">
-        <v>0.1352830198595471</v>
+        <v>2.376663822969495</v>
       </c>
       <c r="V5" t="n">
-        <v>0.05155097081818765</v>
+        <v>2.592424253693962</v>
       </c>
       <c r="W5" t="n">
-        <v>0.09973867328811044</v>
+        <v>3.900903113150885</v>
       </c>
       <c r="X5" t="n">
-        <v>0.04984292570229198</v>
+        <v>2.955490887209062</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.1680626542925896</v>
+        <v>4.403301790244883</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.05157416996268419</v>
+        <v>3.027866510911047</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.07164419693174851</v>
+        <v>2.256805260881249</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.05768569364452938</v>
+        <v>2.543253394995025</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.08950514403305625</v>
+        <v>3.417338753062894</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.07846509541308951</v>
+        <v>2.449897008075816</v>
       </c>
       <c r="AE5" t="n">
-        <v>0.1970189886359818</v>
+        <v>3.982842182560028</v>
       </c>
     </row>
     <row r="6">
@@ -910,94 +910,94 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0761368726809649</v>
+        <v>2.96580115592548</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1063571409170463</v>
+        <v>1.86463661192302</v>
       </c>
       <c r="D6" t="n">
-        <v>0.05236603245060583</v>
+        <v>3.09855209177868</v>
       </c>
       <c r="E6" t="n">
-        <v>0.02768258139341985</v>
+        <v>1.445842074678641</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0.08410375888168144</v>
+        <v>1.703851881076832</v>
       </c>
       <c r="H6" t="n">
-        <v>0.1112220324395065</v>
+        <v>2.310742147204448</v>
       </c>
       <c r="I6" t="n">
-        <v>0.0504172500503835</v>
+        <v>2.53143144480561</v>
       </c>
       <c r="J6" t="n">
-        <v>0.2082216189655968</v>
+        <v>5.581571269578753</v>
       </c>
       <c r="K6" t="n">
-        <v>0.08306929776670594</v>
+        <v>1.9466151879541</v>
       </c>
       <c r="L6" t="n">
-        <v>0.1575374095211401</v>
+        <v>3.128277348035223</v>
       </c>
       <c r="M6" t="n">
-        <v>0.1622277687713889</v>
+        <v>3.622505817627016</v>
       </c>
       <c r="N6" t="n">
-        <v>0.09316152289860903</v>
+        <v>3.840492998543001</v>
       </c>
       <c r="O6" t="n">
-        <v>0.1416074361152511</v>
+        <v>2.589277193548314</v>
       </c>
       <c r="P6" t="n">
-        <v>0.02627434670999546</v>
+        <v>0.7323010431519178</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.1022885784690093</v>
+        <v>2.016848997940187</v>
       </c>
       <c r="R6" t="n">
-        <v>0.05549569324108475</v>
+        <v>1.66481707543581</v>
       </c>
       <c r="S6" t="n">
-        <v>0.05955537797291181</v>
+        <v>1.728056800132495</v>
       </c>
       <c r="T6" t="n">
-        <v>0.1001092886463644</v>
+        <v>2.391902088025556</v>
       </c>
       <c r="U6" t="n">
-        <v>0.1128172584242665</v>
+        <v>1.986473354626657</v>
       </c>
       <c r="V6" t="n">
-        <v>0.04087560208884729</v>
+        <v>1.508085470425701</v>
       </c>
       <c r="W6" t="n">
-        <v>0.1164697180672883</v>
+        <v>3.496330651214064</v>
       </c>
       <c r="X6" t="n">
-        <v>0.03385478775342152</v>
+        <v>2.324685075560781</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.1867814204719543</v>
+        <v>3.797037030146567</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.03870268494845793</v>
+        <v>1.680075056941001</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.04534498745110666</v>
+        <v>1.271772742695402</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.07191582730154523</v>
+        <v>1.523582850402275</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.06263733342079285</v>
+        <v>2.557353822897833</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.05283696998456832</v>
+        <v>1.70533920383869</v>
       </c>
       <c r="AE6" t="n">
-        <v>0.2183983569917965</v>
+        <v>4.184849121853958</v>
       </c>
     </row>
     <row r="7">
@@ -1005,94 +1005,94 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.1500929185360762</v>
+        <v>3.832217408651611</v>
       </c>
       <c r="C7" t="n">
-        <v>0.02583556033628069</v>
+        <v>1.169465854431525</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1094443411160679</v>
+        <v>3.793136514983324</v>
       </c>
       <c r="E7" t="n">
-        <v>0.06248001822044158</v>
+        <v>1.283212431979839</v>
       </c>
       <c r="F7" t="n">
-        <v>0.08410375888168144</v>
+        <v>1.703851881076832</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>0.0433167094672404</v>
+        <v>2.413989225383669</v>
       </c>
       <c r="I7" t="n">
-        <v>0.0889338139040797</v>
+        <v>2.211027557542276</v>
       </c>
       <c r="J7" t="n">
-        <v>0.1250240492275911</v>
+        <v>4.440251440197154</v>
       </c>
       <c r="K7" t="n">
-        <v>0.01322321090755378</v>
+        <v>0.5446389987097822</v>
       </c>
       <c r="L7" t="n">
-        <v>0.07675649465716036</v>
+        <v>2.526792741322411</v>
       </c>
       <c r="M7" t="n">
-        <v>0.08193228683089761</v>
+        <v>3.147284344483641</v>
       </c>
       <c r="N7" t="n">
-        <v>0.1448209632790595</v>
+        <v>4.195271238435983</v>
       </c>
       <c r="O7" t="n">
-        <v>0.05957574506027379</v>
+        <v>1.507612996753175</v>
       </c>
       <c r="P7" t="n">
-        <v>0.07627524710195356</v>
+        <v>1.832428611795925</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.1847419098578239</v>
+        <v>3.649248776787363</v>
       </c>
       <c r="R7" t="n">
-        <v>0.1377539500776272</v>
+        <v>3.24970361777683</v>
       </c>
       <c r="S7" t="n">
-        <v>0.1358737101504976</v>
+        <v>2.365332461944681</v>
       </c>
       <c r="T7" t="n">
-        <v>0.04318045171129105</v>
+        <v>2.722447707839382</v>
       </c>
       <c r="U7" t="n">
-        <v>0.1942288578897537</v>
+        <v>3.32773093726261</v>
       </c>
       <c r="V7" t="n">
-        <v>0.08742127509263364</v>
+        <v>2.358505087950208</v>
       </c>
       <c r="W7" t="n">
-        <v>0.05070744053651875</v>
+        <v>2.926584250984807</v>
       </c>
       <c r="X7" t="n">
-        <v>0.09255668912323532</v>
+        <v>3.346802053074101</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.1067694135644514</v>
+        <v>3.305921909914511</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.0829667021737379</v>
+        <v>2.815801482028545</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.1287128126576745</v>
+        <v>2.813991408063055</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.02733068502701801</v>
+        <v>1.966937345663825</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.1436581071823157</v>
+        <v>3.933073178588527</v>
       </c>
       <c r="AD7" t="n">
-        <v>0.1359434080425483</v>
+        <v>3.10136358871117</v>
       </c>
       <c r="AE7" t="n">
-        <v>0.135194783972139</v>
+        <v>2.750610897135713</v>
       </c>
     </row>
     <row r="8">
@@ -1100,94 +1100,94 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.1676990804217875</v>
+        <v>3.327347127053255</v>
       </c>
       <c r="C8" t="n">
-        <v>0.02890680673827246</v>
+        <v>1.906998640956483</v>
       </c>
       <c r="D8" t="n">
-        <v>0.1386122169166829</v>
+        <v>4.24295364256685</v>
       </c>
       <c r="E8" t="n">
-        <v>0.09484454532190006</v>
+        <v>2.896939806723232</v>
       </c>
       <c r="F8" t="n">
-        <v>0.1112220324395065</v>
+        <v>2.310742147204448</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0433167094672404</v>
+        <v>2.413989225383669</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>0.1271129389457661</v>
+        <v>4.336803367854044</v>
       </c>
       <c r="J8" t="n">
-        <v>0.1113714406046701</v>
+        <v>5.572600470023814</v>
       </c>
       <c r="K8" t="n">
-        <v>0.05444525852849683</v>
+        <v>2.917292810950899</v>
       </c>
       <c r="L8" t="n">
-        <v>0.0554819839681138</v>
+        <v>2.374283730283234</v>
       </c>
       <c r="M8" t="n">
-        <v>0.05956305280838798</v>
+        <v>2.909103826762578</v>
       </c>
       <c r="N8" t="n">
-        <v>0.1778806310777473</v>
+        <v>5.381013953336466</v>
       </c>
       <c r="O8" t="n">
-        <v>0.04045895134114394</v>
+        <v>2.130880151109683</v>
       </c>
       <c r="P8" t="n">
-        <v>0.1060819037291575</v>
+        <v>2.474468958578607</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.2097824875823759</v>
+        <v>3.414956373171784</v>
       </c>
       <c r="R8" t="n">
-        <v>0.1602606449297037</v>
+        <v>2.635472614014816</v>
       </c>
       <c r="S8" t="n">
-        <v>0.1683485879824271</v>
+        <v>3.766040390722482</v>
       </c>
       <c r="T8" t="n">
-        <v>0.04820490715331526</v>
+        <v>2.008958589500698</v>
       </c>
       <c r="U8" t="n">
-        <v>0.2228472832490929</v>
+        <v>3.88284910979623</v>
       </c>
       <c r="V8" t="n">
-        <v>0.1175964105746594</v>
+        <v>2.998096842732995</v>
       </c>
       <c r="W8" t="n">
-        <v>0.06831350358760413</v>
+        <v>4.102141763659696</v>
       </c>
       <c r="X8" t="n">
-        <v>0.1069737984950122</v>
+        <v>2.061539444301041</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.07865944609262772</v>
+        <v>2.435435208114233</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.1076169449191333</v>
+        <v>2.46955197292034</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.152668281102907</v>
+        <v>2.538761578120648</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.0409977708487627</v>
+        <v>1.344213039559745</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.1630230937439195</v>
+        <v>2.862122730740311</v>
       </c>
       <c r="AD8" t="n">
-        <v>0.1581338667132727</v>
+        <v>2.608674232462378</v>
       </c>
       <c r="AE8" t="n">
-        <v>0.1137997480336771</v>
+        <v>3.461875241184558</v>
       </c>
     </row>
     <row r="9">
@@ -1195,94 +1195,94 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.1170792897661876</v>
+        <v>5.00327896930066</v>
       </c>
       <c r="C9" t="n">
-        <v>0.1108070403331864</v>
+        <v>2.774527167876043</v>
       </c>
       <c r="D9" t="n">
-        <v>0.04247425814485747</v>
+        <v>3.324329898372299</v>
       </c>
       <c r="E9" t="n">
-        <v>0.04967780776808293</v>
+        <v>2.229845541437901</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0504172500503835</v>
+        <v>2.53143144480561</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0889338139040797</v>
+        <v>2.211027557542276</v>
       </c>
       <c r="H9" t="n">
-        <v>0.1271129389457661</v>
+        <v>4.336803367854044</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>0.2023608597678263</v>
+        <v>4.648582452213566</v>
       </c>
       <c r="K9" t="n">
-        <v>0.08060728105751409</v>
+        <v>1.774519634539772</v>
       </c>
       <c r="L9" t="n">
-        <v>0.1597331757458119</v>
+        <v>3.885917394419105</v>
       </c>
       <c r="M9" t="n">
-        <v>0.1644428621746648</v>
+        <v>4.283245060141598</v>
       </c>
       <c r="N9" t="n">
-        <v>0.06326772963720222</v>
+        <v>2.819933331980664</v>
       </c>
       <c r="O9" t="n">
-        <v>0.1464564544933867</v>
+        <v>3.252897317460838</v>
       </c>
       <c r="P9" t="n">
-        <v>0.0360632260925678</v>
+        <v>2.338396639413596</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.1149644029762524</v>
+        <v>3.941812926083614</v>
       </c>
       <c r="R9" t="n">
-        <v>0.08274141457612534</v>
+        <v>3.966692272832518</v>
       </c>
       <c r="S9" t="n">
-        <v>0.0588960173870441</v>
+        <v>2.089087094542673</v>
       </c>
       <c r="T9" t="n">
-        <v>0.1013072915979735</v>
+        <v>3.787595281375484</v>
       </c>
       <c r="U9" t="n">
-        <v>0.1178265587005425</v>
+        <v>3.238471068369851</v>
       </c>
       <c r="V9" t="n">
-        <v>0.03272255730527838</v>
+        <v>2.353793982822844</v>
       </c>
       <c r="W9" t="n">
-        <v>0.1034215468999604</v>
+        <v>2.757108656951327</v>
       </c>
       <c r="X9" t="n">
-        <v>0.08311847075483152</v>
+        <v>4.747899255812637</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.1917395403190078</v>
+        <v>4.863815223135096</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.04880611180630125</v>
+        <v>3.38445080783804</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.07456423046973475</v>
+        <v>3.581523944900341</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.08825400647815823</v>
+        <v>3.386952358182625</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.09537928954806282</v>
+        <v>4.908668844500274</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.08567135848253715</v>
+        <v>4.014706852493398</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.2187423493498997</v>
+        <v>4.22249184824608</v>
       </c>
     </row>
     <row r="10">
@@ -1290,94 +1290,94 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.2731512824239208</v>
+        <v>8.178093993708188</v>
       </c>
       <c r="C10" t="n">
-        <v>0.103025345443509</v>
+        <v>3.978835286111829</v>
       </c>
       <c r="D10" t="n">
-        <v>0.2225502853898075</v>
+        <v>4.884540589621968</v>
       </c>
       <c r="E10" t="n">
-        <v>0.1869129579960482</v>
+        <v>5.615539234913368</v>
       </c>
       <c r="F10" t="n">
-        <v>0.2082216189655968</v>
+        <v>5.581571269578753</v>
       </c>
       <c r="G10" t="n">
-        <v>0.1250240492275911</v>
+        <v>4.440251440197154</v>
       </c>
       <c r="H10" t="n">
-        <v>0.1113714406046701</v>
+        <v>5.572600470023814</v>
       </c>
       <c r="I10" t="n">
-        <v>0.2023608597678263</v>
+        <v>4.648582452213566</v>
       </c>
       <c r="J10" t="n">
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>0.1267347225043017</v>
+        <v>4.303653312667597</v>
       </c>
       <c r="L10" t="n">
-        <v>0.05739643763393804</v>
+        <v>3.356668207045927</v>
       </c>
       <c r="M10" t="n">
-        <v>0.05461916936100694</v>
+        <v>3.187098704076983</v>
       </c>
       <c r="N10" t="n">
-        <v>0.2495782195237752</v>
+        <v>4.826495203290631</v>
       </c>
       <c r="O10" t="n">
-        <v>0.0722359682473267</v>
+        <v>3.555365885534079</v>
       </c>
       <c r="P10" t="n">
-        <v>0.1960397329665671</v>
+        <v>5.242531449318038</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.3062531662783816</v>
+        <v>7.344277209721159</v>
       </c>
       <c r="R10" t="n">
-        <v>0.2600442336644484</v>
+        <v>6.908144187316651</v>
       </c>
       <c r="S10" t="n">
-        <v>0.2568831823996444</v>
+        <v>6.324713414454397</v>
       </c>
       <c r="T10" t="n">
-        <v>0.1195797423483573</v>
+        <v>4.704711514179065</v>
       </c>
       <c r="U10" t="n">
-        <v>0.3156312750761827</v>
+        <v>7.278225363830045</v>
       </c>
       <c r="V10" t="n">
-        <v>0.2022559779087088</v>
+        <v>4.991492433366553</v>
       </c>
       <c r="W10" t="n">
-        <v>0.1037425367117263</v>
+        <v>2.584453310344512</v>
       </c>
       <c r="X10" t="n">
-        <v>0.2136556111732859</v>
+        <v>7.307375887821482</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.04758213546145978</v>
+        <v>3.863885889324671</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.1981674589814975</v>
+        <v>5.555508771377668</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.2519989740757531</v>
+        <v>6.751193815342231</v>
       </c>
       <c r="AB10" t="n">
-        <v>0.1407763291467648</v>
+        <v>4.921716305777493</v>
       </c>
       <c r="AC10" t="n">
-        <v>0.2658353880051486</v>
+        <v>7.801804017879788</v>
       </c>
       <c r="AD10" t="n">
-        <v>0.2597030811356905</v>
+        <v>7.173335204743243</v>
       </c>
       <c r="AE10" t="n">
-        <v>0.03095435531326302</v>
+        <v>2.787482330431697</v>
       </c>
     </row>
     <row r="11">
@@ -1385,94 +1385,94 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.1526425676485503</v>
+        <v>4.157587822854066</v>
       </c>
       <c r="C11" t="n">
-        <v>0.03219421679668644</v>
+        <v>1.49285728833284</v>
       </c>
       <c r="D11" t="n">
-        <v>0.103272425056116</v>
+        <v>3.780850335825918</v>
       </c>
       <c r="E11" t="n">
-        <v>0.06144914692949361</v>
+        <v>1.358322179448296</v>
       </c>
       <c r="F11" t="n">
-        <v>0.08306929776670594</v>
+        <v>1.9466151879541</v>
       </c>
       <c r="G11" t="n">
-        <v>0.01322321090755378</v>
+        <v>0.5446389987097822</v>
       </c>
       <c r="H11" t="n">
-        <v>0.05444525852849683</v>
+        <v>2.917292810950899</v>
       </c>
       <c r="I11" t="n">
-        <v>0.08060728105751409</v>
+        <v>1.774519634539772</v>
       </c>
       <c r="J11" t="n">
-        <v>0.1267347225043017</v>
+        <v>4.303653312667597</v>
       </c>
       <c r="K11" t="n">
         <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>0.08132297493744831</v>
+        <v>2.781491568524041</v>
       </c>
       <c r="M11" t="n">
-        <v>0.08642891621714054</v>
+        <v>3.366801904608408</v>
       </c>
       <c r="N11" t="n">
-        <v>0.1359952261153591</v>
+        <v>3.955817443792951</v>
       </c>
       <c r="O11" t="n">
-        <v>0.06612209254273271</v>
+        <v>1.817456210516499</v>
       </c>
       <c r="P11" t="n">
-        <v>0.07208772059785853</v>
+        <v>1.973049067076543</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.1817151650613535</v>
+        <v>3.835195360805996</v>
       </c>
       <c r="R11" t="n">
-        <v>0.1362855666203101</v>
+        <v>3.533701253393235</v>
       </c>
       <c r="S11" t="n">
-        <v>0.131075175738799</v>
+        <v>2.260727266569971</v>
       </c>
       <c r="T11" t="n">
-        <v>0.04256269175568602</v>
+        <v>2.995485259188034</v>
       </c>
       <c r="U11" t="n">
-        <v>0.1901798132192137</v>
+        <v>3.374675933670356</v>
       </c>
       <c r="V11" t="n">
-        <v>0.08138675632370569</v>
+        <v>2.395969081731689</v>
       </c>
       <c r="W11" t="n">
-        <v>0.0435723321353472</v>
+        <v>2.767004934487564</v>
       </c>
       <c r="X11" t="n">
-        <v>0.09587401102562401</v>
+        <v>3.758482226017929</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.1126023542305641</v>
+        <v>3.639812296398546</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.07913716203808327</v>
+        <v>3.032039790480433</v>
       </c>
       <c r="AA11" t="n">
-        <v>0.1272818106757521</v>
+        <v>3.084375166557323</v>
       </c>
       <c r="AB11" t="n">
-        <v>0.03447766186165483</v>
+        <v>2.366146447410879</v>
       </c>
       <c r="AC11" t="n">
-        <v>0.1433635878474069</v>
+        <v>4.267499655479162</v>
       </c>
       <c r="AD11" t="n">
-        <v>0.1354004383445294</v>
+        <v>3.404176755905457</v>
       </c>
       <c r="AE11" t="n">
-        <v>0.1396224029375165</v>
+        <v>2.867477162477153</v>
       </c>
     </row>
     <row r="12">
@@ -1480,94 +1480,94 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.2206008644122393</v>
+        <v>5.412135499019779</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0517059847305083</v>
+        <v>1.428777426463639</v>
       </c>
       <c r="D12" t="n">
-        <v>0.1751484668589876</v>
+        <v>3.358405354585214</v>
       </c>
       <c r="E12" t="n">
-        <v>0.1386683020797322</v>
+        <v>3.679437396973325</v>
       </c>
       <c r="F12" t="n">
-        <v>0.1575374095211401</v>
+        <v>3.128277348035223</v>
       </c>
       <c r="G12" t="n">
-        <v>0.07675649465716036</v>
+        <v>2.526792741322411</v>
       </c>
       <c r="H12" t="n">
-        <v>0.0554819839681138</v>
+        <v>2.374283730283234</v>
       </c>
       <c r="I12" t="n">
-        <v>0.1597331757458119</v>
+        <v>3.885917394419105</v>
       </c>
       <c r="J12" t="n">
-        <v>0.05739643763393804</v>
+        <v>3.356668207045927</v>
       </c>
       <c r="K12" t="n">
-        <v>0.08132297493744831</v>
+        <v>2.781491568524041</v>
       </c>
       <c r="L12" t="n">
         <v>0</v>
       </c>
       <c r="M12" t="n">
-        <v>0.005542336425020126</v>
+        <v>0.6924211871533749</v>
       </c>
       <c r="N12" t="n">
-        <v>0.2077151976504773</v>
+        <v>4.30291400442246</v>
       </c>
       <c r="O12" t="n">
-        <v>0.0228518698921293</v>
+        <v>1.213340057805329</v>
       </c>
       <c r="P12" t="n">
-        <v>0.1466994658128148</v>
+        <v>2.850997822589823</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.2555161863552852</v>
+        <v>4.679117365004681</v>
       </c>
       <c r="R12" t="n">
-        <v>0.2077797609365193</v>
+        <v>4.038623300069887</v>
       </c>
       <c r="S12" t="n">
-        <v>0.2100613198595203</v>
+        <v>4.502611796307393</v>
       </c>
       <c r="T12" t="n">
-        <v>0.068462533651738</v>
+        <v>1.666486036286835</v>
       </c>
       <c r="U12" t="n">
-        <v>0.266988219650689</v>
+        <v>5.009625023984913</v>
       </c>
       <c r="V12" t="n">
-        <v>0.1544133739390624</v>
+        <v>2.835121796382464</v>
       </c>
       <c r="W12" t="n">
-        <v>0.06586915371418693</v>
+        <v>2.251554274048607</v>
       </c>
       <c r="X12" t="n">
-        <v>0.1591848790030104</v>
+        <v>4.222584733571623</v>
       </c>
       <c r="Y12" t="n">
-        <v>0.03247173365975001</v>
+        <v>1.008200803432199</v>
       </c>
       <c r="Z12" t="n">
-        <v>0.1475424493702578</v>
+        <v>2.820034553832355</v>
       </c>
       <c r="AA12" t="n">
-        <v>0.2002507290216913</v>
+        <v>3.994630997121353</v>
       </c>
       <c r="AB12" t="n">
-        <v>0.08693046847478607</v>
+        <v>1.878451524076348</v>
       </c>
       <c r="AC12" t="n">
-        <v>0.2123699603631284</v>
+        <v>4.754534625479854</v>
       </c>
       <c r="AD12" t="n">
-        <v>0.2072976474389855</v>
+        <v>4.339606747773769</v>
       </c>
       <c r="AE12" t="n">
-        <v>0.06471658377099473</v>
+        <v>2.097788228018719</v>
       </c>
     </row>
     <row r="13">
@@ -1575,94 +1575,94 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.2252101835970057</v>
+        <v>5.982288785562577</v>
       </c>
       <c r="C13" t="n">
-        <v>0.05669802497754553</v>
+        <v>2.037703753661898</v>
       </c>
       <c r="D13" t="n">
-        <v>0.1792538855410932</v>
+        <v>3.291429531873295</v>
       </c>
       <c r="E13" t="n">
-        <v>0.1436865963437164</v>
+        <v>4.283590739917385</v>
       </c>
       <c r="F13" t="n">
-        <v>0.1622277687713889</v>
+        <v>3.622505817627016</v>
       </c>
       <c r="G13" t="n">
-        <v>0.08193228683089761</v>
+        <v>3.147284344483641</v>
       </c>
       <c r="H13" t="n">
-        <v>0.05956305280838798</v>
+        <v>2.909103826762578</v>
       </c>
       <c r="I13" t="n">
-        <v>0.1644428621746648</v>
+        <v>4.283245060141598</v>
       </c>
       <c r="J13" t="n">
-        <v>0.05461916936100694</v>
+        <v>3.187098704076983</v>
       </c>
       <c r="K13" t="n">
-        <v>0.08642891621714054</v>
+        <v>3.366801904608408</v>
       </c>
       <c r="L13" t="n">
-        <v>0.005542336425020126</v>
+        <v>0.6924211871533749</v>
       </c>
       <c r="M13" t="n">
         <v>0</v>
       </c>
       <c r="N13" t="n">
-        <v>0.2117176405575271</v>
+        <v>4.301643548146136</v>
       </c>
       <c r="O13" t="n">
-        <v>0.02788487592237225</v>
+        <v>1.842011803911781</v>
       </c>
       <c r="P13" t="n">
-        <v>0.15120032007019</v>
+        <v>3.288510111057312</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.2598442911965493</v>
+        <v>5.064367124393922</v>
       </c>
       <c r="R13" t="n">
-        <v>0.2121107779011778</v>
+        <v>4.430820966659384</v>
       </c>
       <c r="S13" t="n">
-        <v>0.2148019152534487</v>
+        <v>5.03205764722014</v>
       </c>
       <c r="T13" t="n">
-        <v>0.07203290561140487</v>
+        <v>1.906825919579325</v>
       </c>
       <c r="U13" t="n">
-        <v>0.2715104821632445</v>
+        <v>5.481457593136255</v>
       </c>
       <c r="V13" t="n">
-        <v>0.1587011230038706</v>
+        <v>3.130652564540006</v>
       </c>
       <c r="W13" t="n">
-        <v>0.06949785456299067</v>
+        <v>2.254483704351522</v>
       </c>
       <c r="X13" t="n">
-        <v>0.1635362526013421</v>
+        <v>4.725646503799299</v>
       </c>
       <c r="Y13" t="n">
-        <v>0.02837070400902465</v>
+        <v>1.014751470146016</v>
       </c>
       <c r="Z13" t="n">
-        <v>0.1516576549637516</v>
+        <v>3.086620502949681</v>
       </c>
       <c r="AA13" t="n">
-        <v>0.2047260776834877</v>
+        <v>4.460909353845585</v>
       </c>
       <c r="AB13" t="n">
-        <v>0.09141891301050482</v>
+        <v>2.335110092897443</v>
       </c>
       <c r="AC13" t="n">
-        <v>0.2166223082488395</v>
+        <v>5.187096518951847</v>
       </c>
       <c r="AD13" t="n">
-        <v>0.2117784626108641</v>
+        <v>4.830246499010525</v>
       </c>
       <c r="AE13" t="n">
-        <v>0.06159353181354079</v>
+        <v>2.459343166866641</v>
       </c>
     </row>
     <row r="14">
@@ -1670,94 +1670,94 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>0.1398273506350843</v>
+        <v>6.649882146058538</v>
       </c>
       <c r="C14" t="n">
-        <v>0.1626016982039385</v>
+        <v>3.920272848881794</v>
       </c>
       <c r="D14" t="n">
-        <v>0.04569867082713736</v>
+        <v>1.717103940274897</v>
       </c>
       <c r="E14" t="n">
-        <v>0.1066659509039129</v>
+        <v>4.504453589626598</v>
       </c>
       <c r="F14" t="n">
-        <v>0.09316152289860903</v>
+        <v>3.840492998543001</v>
       </c>
       <c r="G14" t="n">
-        <v>0.1448209632790595</v>
+        <v>4.195271238435983</v>
       </c>
       <c r="H14" t="n">
-        <v>0.1778806310777473</v>
+        <v>5.381013953336466</v>
       </c>
       <c r="I14" t="n">
-        <v>0.06326772963720222</v>
+        <v>2.819933331980664</v>
       </c>
       <c r="J14" t="n">
-        <v>0.2495782195237752</v>
+        <v>4.826495203290631</v>
       </c>
       <c r="K14" t="n">
-        <v>0.1359952261153591</v>
+        <v>3.955817443792951</v>
       </c>
       <c r="L14" t="n">
-        <v>0.2077151976504773</v>
+        <v>4.30291400442246</v>
       </c>
       <c r="M14" t="n">
-        <v>0.2117176405575271</v>
+        <v>4.301643548146136</v>
       </c>
       <c r="N14" t="n">
         <v>0</v>
       </c>
       <c r="O14" t="n">
-        <v>0.198570712270195</v>
+        <v>4.469269329325149</v>
       </c>
       <c r="P14" t="n">
-        <v>0.07841968475658202</v>
+        <v>3.243813217558934</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.09342091405528022</v>
+        <v>4.480621065717854</v>
       </c>
       <c r="R14" t="n">
-        <v>0.08633408502987405</v>
+        <v>4.562931023410719</v>
       </c>
       <c r="S14" t="n">
-        <v>0.0640189882101071</v>
+        <v>4.087573172460641</v>
       </c>
       <c r="T14" t="n">
-        <v>0.1428224696317817</v>
+        <v>3.799836642845206</v>
       </c>
       <c r="U14" t="n">
-        <v>0.09380339107608786</v>
+        <v>4.428297707296855</v>
       </c>
       <c r="V14" t="n">
-        <v>0.06274080834460957</v>
+        <v>2.51508863156435</v>
       </c>
       <c r="W14" t="n">
-        <v>0.1463375744119478</v>
+        <v>2.536755405230279</v>
       </c>
       <c r="X14" t="n">
-        <v>0.1189611972094547</v>
+        <v>5.877434064007069</v>
       </c>
       <c r="Y14" t="n">
-        <v>0.2397047406442568</v>
+        <v>5.177568356281527</v>
       </c>
       <c r="Z14" t="n">
-        <v>0.07676070911372927</v>
+        <v>3.364356727353928</v>
       </c>
       <c r="AA14" t="n">
-        <v>0.08625198607646963</v>
+        <v>4.578672254166672</v>
       </c>
       <c r="AB14" t="n">
-        <v>0.138573059310039</v>
+        <v>4.089424653742001</v>
       </c>
       <c r="AC14" t="n">
-        <v>0.09984792019169891</v>
+        <v>5.685022832115944</v>
       </c>
       <c r="AD14" t="n">
-        <v>0.09726082461286675</v>
+        <v>5.134173783153908</v>
       </c>
       <c r="AE14" t="n">
-        <v>0.2686522967267873</v>
+        <v>5.481667918899217</v>
       </c>
     </row>
     <row r="15">
@@ -1765,94 +1765,94 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.2025138145825583</v>
+        <v>4.738182926070425</v>
       </c>
       <c r="C15" t="n">
-        <v>0.03688028570382887</v>
+        <v>0.8161055600022139</v>
       </c>
       <c r="D15" t="n">
-        <v>0.1643767192334777</v>
+        <v>3.760408479238031</v>
       </c>
       <c r="E15" t="n">
-        <v>0.1211374580608665</v>
+        <v>2.731175742241764</v>
       </c>
       <c r="F15" t="n">
-        <v>0.1416074361152511</v>
+        <v>2.589277193548314</v>
       </c>
       <c r="G15" t="n">
-        <v>0.05957574506027379</v>
+        <v>1.507612996753175</v>
       </c>
       <c r="H15" t="n">
-        <v>0.04045895134114394</v>
+        <v>2.130880151109683</v>
       </c>
       <c r="I15" t="n">
-        <v>0.1464564544933867</v>
+        <v>3.252897317460838</v>
       </c>
       <c r="J15" t="n">
-        <v>0.0722359682473267</v>
+        <v>3.555365885534079</v>
       </c>
       <c r="K15" t="n">
-        <v>0.06612209254273271</v>
+        <v>1.817456210516499</v>
       </c>
       <c r="L15" t="n">
-        <v>0.0228518698921293</v>
+        <v>1.213340057805329</v>
       </c>
       <c r="M15" t="n">
-        <v>0.02788487592237225</v>
+        <v>1.842011803911781</v>
       </c>
       <c r="N15" t="n">
-        <v>0.198570712270195</v>
+        <v>4.469269329325149</v>
       </c>
       <c r="O15" t="n">
         <v>0</v>
       </c>
       <c r="P15" t="n">
-        <v>0.1333525746322962</v>
+        <v>2.524859879697706</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.241785953894931</v>
+        <v>4.438979762287582</v>
       </c>
       <c r="R15" t="n">
-        <v>0.1935700279760278</v>
+        <v>3.841252964481239</v>
       </c>
       <c r="S15" t="n">
-        <v>0.1951173006547773</v>
+        <v>3.763553506568592</v>
       </c>
       <c r="T15" t="n">
-        <v>0.06346050344248656</v>
+        <v>2.217249154278552</v>
       </c>
       <c r="U15" t="n">
-        <v>0.252692322502249</v>
+        <v>4.496913142892707</v>
       </c>
       <c r="V15" t="n">
-        <v>0.1429167696077333</v>
+        <v>2.784188151829227</v>
       </c>
       <c r="W15" t="n">
-        <v>0.0632800353510565</v>
+        <v>2.507313357982912</v>
       </c>
       <c r="X15" t="n">
-        <v>0.1433053590036265</v>
+        <v>3.848829194791297</v>
       </c>
       <c r="Y15" t="n">
-        <v>0.048146010899878</v>
+        <v>1.913281079604493</v>
       </c>
       <c r="Z15" t="n">
-        <v>0.1363391253771885</v>
+        <v>2.974758535670767</v>
       </c>
       <c r="AA15" t="n">
-        <v>0.1853172733942032</v>
+        <v>3.609283516669732</v>
       </c>
       <c r="AB15" t="n">
-        <v>0.07221681081132462</v>
+        <v>1.78930682713557</v>
       </c>
       <c r="AC15" t="n">
-        <v>0.1979948880899807</v>
+        <v>4.515381444009831</v>
       </c>
       <c r="AD15" t="n">
-        <v>0.1918565697619008</v>
+        <v>3.906025157657836</v>
       </c>
       <c r="AE15" t="n">
-        <v>0.07704689741252965</v>
+        <v>1.664699071974984</v>
       </c>
     </row>
     <row r="16">
@@ -1860,94 +1860,94 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0.1004080704858452</v>
+        <v>3.561225118834551</v>
       </c>
       <c r="C16" t="n">
-        <v>0.09663050145433673</v>
+        <v>1.719034027001325</v>
       </c>
       <c r="D16" t="n">
-        <v>0.03672827384948462</v>
+        <v>2.502264969245576</v>
       </c>
       <c r="E16" t="n">
-        <v>0.03530546654983772</v>
+        <v>1.88676867875883</v>
       </c>
       <c r="F16" t="n">
-        <v>0.02627434670999546</v>
+        <v>0.7323010431519178</v>
       </c>
       <c r="G16" t="n">
-        <v>0.07627524710195356</v>
+        <v>1.832428611795925</v>
       </c>
       <c r="H16" t="n">
-        <v>0.1060819037291575</v>
+        <v>2.474468958578607</v>
       </c>
       <c r="I16" t="n">
-        <v>0.0360632260925678</v>
+        <v>2.338396639413596</v>
       </c>
       <c r="J16" t="n">
-        <v>0.1960397329665671</v>
+        <v>5.242531449318038</v>
       </c>
       <c r="K16" t="n">
-        <v>0.07208772059785853</v>
+        <v>1.973049067076543</v>
       </c>
       <c r="L16" t="n">
-        <v>0.1466994658128148</v>
+        <v>2.850997822589823</v>
       </c>
       <c r="M16" t="n">
-        <v>0.15120032007019</v>
+        <v>3.288510111057312</v>
       </c>
       <c r="N16" t="n">
-        <v>0.07841968475658202</v>
+        <v>3.243813217558934</v>
       </c>
       <c r="O16" t="n">
-        <v>0.1333525746322962</v>
+        <v>2.524859879697706</v>
       </c>
       <c r="P16" t="n">
         <v>0</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.110457356965625</v>
+        <v>2.127537534766293</v>
       </c>
       <c r="R16" t="n">
-        <v>0.06686721750176727</v>
+        <v>1.826325880087521</v>
       </c>
       <c r="S16" t="n">
-        <v>0.06547741480863066</v>
+        <v>1.97597868622381</v>
       </c>
       <c r="T16" t="n">
-        <v>0.08417465326952632</v>
+        <v>1.959311234553469</v>
       </c>
       <c r="U16" t="n">
-        <v>0.1205105585980626</v>
+        <v>2.214201427830503</v>
       </c>
       <c r="V16" t="n">
-        <v>0.01754282633670263</v>
+        <v>0.8201268582487746</v>
       </c>
       <c r="W16" t="n">
-        <v>0.09829631881750918</v>
+        <v>2.975092834828807</v>
       </c>
       <c r="X16" t="n">
-        <v>0.05194549270057697</v>
+        <v>2.731135044305354</v>
       </c>
       <c r="Y16" t="n">
-        <v>0.1774060249428374</v>
+        <v>3.596335204532062</v>
       </c>
       <c r="Z16" t="n">
-        <v>0.01842342542976349</v>
+        <v>1.215086795697153</v>
       </c>
       <c r="AA16" t="n">
-        <v>0.05919456782280713</v>
+        <v>1.617213135699892</v>
       </c>
       <c r="AB16" t="n">
-        <v>0.06523550110603832</v>
+        <v>1.4247580709917</v>
       </c>
       <c r="AC16" t="n">
-        <v>0.07630925066796164</v>
+        <v>2.835949959353229</v>
       </c>
       <c r="AD16" t="n">
-        <v>0.06949132193266785</v>
+        <v>2.131754661178397</v>
       </c>
       <c r="AE16" t="n">
-        <v>0.2090424202941703</v>
+        <v>4.102973629951916</v>
       </c>
     </row>
     <row r="17">
@@ -1955,94 +1955,94 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.08550039492222347</v>
+        <v>2.767369523368556</v>
       </c>
       <c r="C17" t="n">
-        <v>0.2056706577428302</v>
+        <v>3.675524341203782</v>
       </c>
       <c r="D17" t="n">
-        <v>0.08989481022093464</v>
+        <v>3.641278611538448</v>
       </c>
       <c r="E17" t="n">
-        <v>0.1274004179708874</v>
+        <v>3.037540912504872</v>
       </c>
       <c r="F17" t="n">
-        <v>0.1022885784690093</v>
+        <v>2.016848997940187</v>
       </c>
       <c r="G17" t="n">
-        <v>0.1847419098578239</v>
+        <v>3.649248776787363</v>
       </c>
       <c r="H17" t="n">
-        <v>0.2097824875823759</v>
+        <v>3.414956373171784</v>
       </c>
       <c r="I17" t="n">
-        <v>0.1149644029762524</v>
+        <v>3.941812926083614</v>
       </c>
       <c r="J17" t="n">
-        <v>0.3062531662783816</v>
+        <v>7.344277209721159</v>
       </c>
       <c r="K17" t="n">
-        <v>0.1817151650613535</v>
+        <v>3.835195360805996</v>
       </c>
       <c r="L17" t="n">
-        <v>0.2555161863552852</v>
+        <v>4.679117365004681</v>
       </c>
       <c r="M17" t="n">
-        <v>0.2598442911965493</v>
+        <v>5.064367124393922</v>
       </c>
       <c r="N17" t="n">
-        <v>0.09342091405528022</v>
+        <v>4.480621065717854</v>
       </c>
       <c r="O17" t="n">
-        <v>0.241785953894931</v>
+        <v>4.438979762287582</v>
       </c>
       <c r="P17" t="n">
-        <v>0.110457356965625</v>
+        <v>2.127537534766293</v>
       </c>
       <c r="Q17" t="n">
         <v>0</v>
       </c>
       <c r="R17" t="n">
-        <v>0.05032919685453657</v>
+        <v>0.8412540570711472</v>
       </c>
       <c r="S17" t="n">
-        <v>0.06073040458344973</v>
+        <v>2.490639442986376</v>
       </c>
       <c r="T17" t="n">
-        <v>0.1912734883271535</v>
+        <v>3.34097670316005</v>
       </c>
       <c r="U17" t="n">
-        <v>0.02466754794895206</v>
+        <v>1.342395342297252</v>
       </c>
       <c r="V17" t="n">
-        <v>0.1064165670858177</v>
+        <v>2.46639243407309</v>
       </c>
       <c r="W17" t="n">
-        <v>0.2072033993866904</v>
+        <v>4.987206341788692</v>
       </c>
       <c r="X17" t="n">
-        <v>0.1093968924166139</v>
+        <v>2.188515595787691</v>
       </c>
       <c r="Y17" t="n">
-        <v>0.2850144760492523</v>
+        <v>5.178911449765597</v>
       </c>
       <c r="Z17" t="n">
-        <v>0.1100084656472157</v>
+        <v>2.099837069023817</v>
       </c>
       <c r="AA17" t="n">
-        <v>0.058512015827461</v>
+        <v>1.014508839393335</v>
       </c>
       <c r="AB17" t="n">
-        <v>0.1704743870869087</v>
+        <v>2.88156214656459</v>
       </c>
       <c r="AC17" t="n">
-        <v>0.05291877158688211</v>
+        <v>1.49367187264913</v>
       </c>
       <c r="AD17" t="n">
-        <v>0.05672623030059108</v>
+        <v>1.239298588369926</v>
       </c>
       <c r="AE17" t="n">
-        <v>0.3182655032197653</v>
+        <v>6.061348784835237</v>
       </c>
     </row>
     <row r="18">
@@ -2050,94 +2050,94 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.05933621753647254</v>
+        <v>2.598761112483388</v>
       </c>
       <c r="C18" t="n">
-        <v>0.1580751883247034</v>
+        <v>3.122229747150397</v>
       </c>
       <c r="D18" t="n">
-        <v>0.05880516976923385</v>
+        <v>3.503876573838752</v>
       </c>
       <c r="E18" t="n">
-        <v>0.08245061718406671</v>
+        <v>2.848295112824452</v>
       </c>
       <c r="F18" t="n">
-        <v>0.05549569324108475</v>
+        <v>1.66481707543581</v>
       </c>
       <c r="G18" t="n">
-        <v>0.1377539500776272</v>
+        <v>3.24970361777683</v>
       </c>
       <c r="H18" t="n">
-        <v>0.1602606449297037</v>
+        <v>2.635472614014816</v>
       </c>
       <c r="I18" t="n">
-        <v>0.08274141457612534</v>
+        <v>3.966692272832518</v>
       </c>
       <c r="J18" t="n">
-        <v>0.2600442336644484</v>
+        <v>6.908144187316651</v>
       </c>
       <c r="K18" t="n">
-        <v>0.1362855666203101</v>
+        <v>3.533701253393235</v>
       </c>
       <c r="L18" t="n">
-        <v>0.2077797609365193</v>
+        <v>4.038623300069887</v>
       </c>
       <c r="M18" t="n">
-        <v>0.2121107779011778</v>
+        <v>4.430820966659384</v>
       </c>
       <c r="N18" t="n">
-        <v>0.08633408502987405</v>
+        <v>4.562931023410719</v>
       </c>
       <c r="O18" t="n">
-        <v>0.1935700279760278</v>
+        <v>3.841252964481239</v>
       </c>
       <c r="P18" t="n">
-        <v>0.06686721750176727</v>
+        <v>1.826325880087521</v>
       </c>
       <c r="Q18" t="n">
-        <v>0.05032919685453657</v>
+        <v>0.8412540570711472</v>
       </c>
       <c r="R18" t="n">
         <v>0</v>
       </c>
       <c r="S18" t="n">
-        <v>0.0451855892448829</v>
+        <v>2.686604806024552</v>
       </c>
       <c r="T18" t="n">
-        <v>0.1453814740049664</v>
+        <v>2.728105054080145</v>
       </c>
       <c r="U18" t="n">
-        <v>0.06738817356617736</v>
+        <v>1.880894365876595</v>
       </c>
       <c r="V18" t="n">
-        <v>0.06789922186111755</v>
+        <v>2.261771904967924</v>
       </c>
       <c r="W18" t="n">
-        <v>0.1642773486842691</v>
+        <v>4.66810129394759</v>
       </c>
       <c r="X18" t="n">
-        <v>0.05957146884096129</v>
+        <v>1.601082265043603</v>
       </c>
       <c r="Y18" t="n">
-        <v>0.2364994698977393</v>
+        <v>4.449983453728541</v>
       </c>
       <c r="Z18" t="n">
-        <v>0.06684733808302573</v>
+        <v>1.647103031328638</v>
       </c>
       <c r="AA18" t="n">
-        <v>0.01202558997330699</v>
+        <v>0.6506224729803936</v>
       </c>
       <c r="AB18" t="n">
-        <v>0.1217163835627062</v>
+        <v>2.193384957508877</v>
       </c>
       <c r="AC18" t="n">
-        <v>0.01441431731969894</v>
+        <v>1.165778089047655</v>
       </c>
       <c r="AD18" t="n">
-        <v>0.01495660068341693</v>
+        <v>0.9286345308215204</v>
       </c>
       <c r="AE18" t="n">
-        <v>0.2703665663826597</v>
+        <v>5.475393427086924</v>
       </c>
     </row>
     <row r="19">
@@ -2145,94 +2145,94 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>0.08154452064721616</v>
+        <v>3.14790077987135</v>
       </c>
       <c r="C19" t="n">
-        <v>0.1590478083411667</v>
+        <v>3.117626289337508</v>
       </c>
       <c r="D19" t="n">
-        <v>0.05333489253446617</v>
+        <v>4.021480431751958</v>
       </c>
       <c r="E19" t="n">
-        <v>0.07760526225878886</v>
+        <v>1.332068341822178</v>
       </c>
       <c r="F19" t="n">
-        <v>0.05955537797291181</v>
+        <v>1.728056800132495</v>
       </c>
       <c r="G19" t="n">
-        <v>0.1358737101504976</v>
+        <v>2.365332461944681</v>
       </c>
       <c r="H19" t="n">
-        <v>0.1683485879824271</v>
+        <v>3.766040390722482</v>
       </c>
       <c r="I19" t="n">
-        <v>0.0588960173870441</v>
+        <v>2.089087094542673</v>
       </c>
       <c r="J19" t="n">
-        <v>0.2568831823996444</v>
+        <v>6.324713414454397</v>
       </c>
       <c r="K19" t="n">
-        <v>0.131075175738799</v>
+        <v>2.260727266569971</v>
       </c>
       <c r="L19" t="n">
-        <v>0.2100613198595203</v>
+        <v>4.502611796307393</v>
       </c>
       <c r="M19" t="n">
-        <v>0.2148019152534487</v>
+        <v>5.03205764722014</v>
       </c>
       <c r="N19" t="n">
-        <v>0.0640189882101071</v>
+        <v>4.087573172460641</v>
       </c>
       <c r="O19" t="n">
-        <v>0.1951173006547773</v>
+        <v>3.763553506568592</v>
       </c>
       <c r="P19" t="n">
-        <v>0.06547741480863066</v>
+        <v>1.97597868622381</v>
       </c>
       <c r="Q19" t="n">
-        <v>0.06073040458344973</v>
+        <v>2.490639442986376</v>
       </c>
       <c r="R19" t="n">
-        <v>0.0451855892448829</v>
+        <v>2.686604806024552</v>
       </c>
       <c r="S19" t="n">
         <v>0</v>
       </c>
       <c r="T19" t="n">
-        <v>0.1491434771829654</v>
+        <v>3.874467096129107</v>
       </c>
       <c r="U19" t="n">
-        <v>0.06095264082284668</v>
+        <v>1.416068152163214</v>
       </c>
       <c r="V19" t="n">
-        <v>0.06309385098344696</v>
+        <v>2.500159364299273</v>
       </c>
       <c r="W19" t="n">
-        <v>0.1587973020634575</v>
+        <v>4.26411015053906</v>
       </c>
       <c r="X19" t="n">
-        <v>0.08300995717850779</v>
+        <v>3.282453765497387</v>
       </c>
       <c r="Y19" t="n">
-        <v>0.2408986538741369</v>
+        <v>5.292281537201471</v>
       </c>
       <c r="Z19" t="n">
-        <v>0.07325439192003551</v>
+        <v>3.052157723170735</v>
       </c>
       <c r="AA19" t="n">
-        <v>0.0399551997674322</v>
+        <v>2.13799710751497</v>
       </c>
       <c r="AB19" t="n">
-        <v>0.1280817178360158</v>
+        <v>3.172784562222847</v>
       </c>
       <c r="AC19" t="n">
-        <v>0.05821637843368258</v>
+        <v>3.33475331197733</v>
       </c>
       <c r="AD19" t="n">
-        <v>0.04766195734996809</v>
+        <v>2.394412596012076</v>
       </c>
       <c r="AE19" t="n">
-        <v>0.2704513459680312</v>
+        <v>5.088489688151256</v>
       </c>
     </row>
     <row r="20">
@@ -2240,94 +2240,94 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>0.1695531917721534</v>
+        <v>4.634872707588587</v>
       </c>
       <c r="C20" t="n">
-        <v>0.03447710624140341</v>
+        <v>1.711905118640308</v>
       </c>
       <c r="D20" t="n">
-        <v>0.1090201844341099</v>
+        <v>2.546009891248666</v>
       </c>
       <c r="E20" t="n">
-        <v>0.08789601675861024</v>
+        <v>3.436736765950698</v>
       </c>
       <c r="F20" t="n">
-        <v>0.1001092886463644</v>
+        <v>2.391902088025556</v>
       </c>
       <c r="G20" t="n">
-        <v>0.04318045171129105</v>
+        <v>2.722447707839382</v>
       </c>
       <c r="H20" t="n">
-        <v>0.04820490715331526</v>
+        <v>2.008958589500698</v>
       </c>
       <c r="I20" t="n">
-        <v>0.1013072915979735</v>
+        <v>3.787595281375484</v>
       </c>
       <c r="J20" t="n">
-        <v>0.1195797423483573</v>
+        <v>4.704711514179065</v>
       </c>
       <c r="K20" t="n">
-        <v>0.04256269175568602</v>
+        <v>2.995485259188034</v>
       </c>
       <c r="L20" t="n">
-        <v>0.068462533651738</v>
+        <v>1.666486036286835</v>
       </c>
       <c r="M20" t="n">
-        <v>0.07203290561140487</v>
+        <v>1.906825919579325</v>
       </c>
       <c r="N20" t="n">
-        <v>0.1428224696317817</v>
+        <v>3.799836642845206</v>
       </c>
       <c r="O20" t="n">
-        <v>0.06346050344248656</v>
+        <v>2.217249154278552</v>
       </c>
       <c r="P20" t="n">
-        <v>0.08417465326952632</v>
+        <v>1.959311234553469</v>
       </c>
       <c r="Q20" t="n">
-        <v>0.1912734883271535</v>
+        <v>3.34097670316005</v>
       </c>
       <c r="R20" t="n">
-        <v>0.1453814740049664</v>
+        <v>2.728105054080145</v>
       </c>
       <c r="S20" t="n">
-        <v>0.1491434771829654</v>
+        <v>3.874467096129107</v>
       </c>
       <c r="T20" t="n">
         <v>0</v>
       </c>
       <c r="U20" t="n">
-        <v>0.2034586964705716</v>
+        <v>3.951604100213009</v>
       </c>
       <c r="V20" t="n">
-        <v>0.08930657052804938</v>
+        <v>1.858798124552481</v>
       </c>
       <c r="W20" t="n">
-        <v>0.03502579071543321</v>
+        <v>2.737587857702662</v>
       </c>
       <c r="X20" t="n">
-        <v>0.1053349215250191</v>
+        <v>3.243077592389029</v>
       </c>
       <c r="Y20" t="n">
-        <v>0.09880706708484376</v>
+        <v>2.09242044539375</v>
       </c>
       <c r="Z20" t="n">
-        <v>0.08155459011418004</v>
+        <v>1.368953100373821</v>
       </c>
       <c r="AA20" t="n">
-        <v>0.1391026047535804</v>
+        <v>2.86672296401834</v>
       </c>
       <c r="AB20" t="n">
-        <v>0.03929662516899492</v>
+        <v>1.153107146047482</v>
       </c>
       <c r="AC20" t="n">
-        <v>0.1511139983226706</v>
+        <v>3.482268086760989</v>
       </c>
       <c r="AD20" t="n">
-        <v>0.1474567957062103</v>
+        <v>3.251018594262992</v>
       </c>
       <c r="AE20" t="n">
-        <v>0.1327338608457503</v>
+        <v>3.595147026549128</v>
       </c>
     </row>
     <row r="21">
@@ -2335,94 +2335,94 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>0.09699225377234293</v>
+        <v>2.695516964504267</v>
       </c>
       <c r="C21" t="n">
-        <v>0.2164221395242461</v>
+        <v>3.755023586331237</v>
       </c>
       <c r="D21" t="n">
-        <v>0.09906558595463066</v>
+        <v>4.056942536646842</v>
       </c>
       <c r="E21" t="n">
-        <v>0.1352830198595471</v>
+        <v>2.376663822969495</v>
       </c>
       <c r="F21" t="n">
-        <v>0.1128172584242665</v>
+        <v>1.986473354626657</v>
       </c>
       <c r="G21" t="n">
-        <v>0.1942288578897537</v>
+        <v>3.32773093726261</v>
       </c>
       <c r="H21" t="n">
-        <v>0.2228472832490929</v>
+        <v>3.88284910979623</v>
       </c>
       <c r="I21" t="n">
-        <v>0.1178265587005425</v>
+        <v>3.238471068369851</v>
       </c>
       <c r="J21" t="n">
-        <v>0.3156312750761827</v>
+        <v>7.278225363830045</v>
       </c>
       <c r="K21" t="n">
-        <v>0.1901798132192137</v>
+        <v>3.374675933670356</v>
       </c>
       <c r="L21" t="n">
-        <v>0.266988219650689</v>
+        <v>5.009625023984913</v>
       </c>
       <c r="M21" t="n">
-        <v>0.2715104821632445</v>
+        <v>5.481457593136255</v>
       </c>
       <c r="N21" t="n">
-        <v>0.09380339107608786</v>
+        <v>4.428297707296855</v>
       </c>
       <c r="O21" t="n">
-        <v>0.252692322502249</v>
+        <v>4.496913142892707</v>
       </c>
       <c r="P21" t="n">
-        <v>0.1205105585980626</v>
+        <v>2.214201427830503</v>
       </c>
       <c r="Q21" t="n">
-        <v>0.02466754794895206</v>
+        <v>1.342395342297252</v>
       </c>
       <c r="R21" t="n">
-        <v>0.06738817356617736</v>
+        <v>1.880894365876595</v>
       </c>
       <c r="S21" t="n">
-        <v>0.06095264082284668</v>
+        <v>1.416068152163214</v>
       </c>
       <c r="T21" t="n">
-        <v>0.2034586964705716</v>
+        <v>3.951604100213009</v>
       </c>
       <c r="U21" t="n">
         <v>0</v>
       </c>
       <c r="V21" t="n">
-        <v>0.1157790163405195</v>
+        <v>2.669554751967458</v>
       </c>
       <c r="W21" t="n">
-        <v>0.2160186059144839</v>
+        <v>4.992074112235162</v>
       </c>
       <c r="X21" t="n">
-        <v>0.1249036799493486</v>
+        <v>2.761215662975023</v>
       </c>
       <c r="Y21" t="n">
-        <v>0.2972676261132158</v>
+        <v>5.669229892955243</v>
       </c>
       <c r="Z21" t="n">
-        <v>0.1226115853716651</v>
+        <v>2.813572345407069</v>
       </c>
       <c r="AA21" t="n">
-        <v>0.07256016988428485</v>
+        <v>1.503997662167468</v>
       </c>
       <c r="AB21" t="n">
-        <v>0.1828658026562699</v>
+        <v>3.342572875309702</v>
       </c>
       <c r="AC21" t="n">
-        <v>0.07246672653759842</v>
+        <v>2.392409977351756</v>
       </c>
       <c r="AD21" t="n">
-        <v>0.07184335996326389</v>
+        <v>1.678718479843614</v>
       </c>
       <c r="AE21" t="n">
-        <v>0.3287483354548894</v>
+        <v>6.007126894520279</v>
       </c>
     </row>
     <row r="22">
@@ -2430,94 +2430,94 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>0.1101634197502209</v>
+        <v>4.31965444962708</v>
       </c>
       <c r="C22" t="n">
-        <v>0.1060777649125607</v>
+        <v>2.004260683280279</v>
       </c>
       <c r="D22" t="n">
-        <v>0.0223858684056301</v>
+        <v>1.72120595170779</v>
       </c>
       <c r="E22" t="n">
-        <v>0.05155097081818765</v>
+        <v>2.592424253693962</v>
       </c>
       <c r="F22" t="n">
-        <v>0.04087560208884729</v>
+        <v>1.508085470425701</v>
       </c>
       <c r="G22" t="n">
-        <v>0.08742127509263364</v>
+        <v>2.358505087950208</v>
       </c>
       <c r="H22" t="n">
-        <v>0.1175964105746594</v>
+        <v>2.998096842732995</v>
       </c>
       <c r="I22" t="n">
-        <v>0.03272255730527838</v>
+        <v>2.353793982822844</v>
       </c>
       <c r="J22" t="n">
-        <v>0.2022559779087088</v>
+        <v>4.991492433366553</v>
       </c>
       <c r="K22" t="n">
-        <v>0.08138675632370569</v>
+        <v>2.395969081731689</v>
       </c>
       <c r="L22" t="n">
-        <v>0.1544133739390624</v>
+        <v>2.835121796382464</v>
       </c>
       <c r="M22" t="n">
-        <v>0.1587011230038706</v>
+        <v>3.130652564540006</v>
       </c>
       <c r="N22" t="n">
-        <v>0.06274080834460957</v>
+        <v>2.51508863156435</v>
       </c>
       <c r="O22" t="n">
-        <v>0.1429167696077333</v>
+        <v>2.784188151829227</v>
       </c>
       <c r="P22" t="n">
-        <v>0.01754282633670263</v>
+        <v>0.8201268582487746</v>
       </c>
       <c r="Q22" t="n">
-        <v>0.1064165670858177</v>
+        <v>2.46639243407309</v>
       </c>
       <c r="R22" t="n">
-        <v>0.06789922186111755</v>
+        <v>2.261771904967924</v>
       </c>
       <c r="S22" t="n">
-        <v>0.06309385098344696</v>
+        <v>2.500159364299273</v>
       </c>
       <c r="T22" t="n">
-        <v>0.08930657052804938</v>
+        <v>1.858798124552481</v>
       </c>
       <c r="U22" t="n">
-        <v>0.1157790163405195</v>
+        <v>2.669554751967458</v>
       </c>
       <c r="V22" t="n">
         <v>0</v>
       </c>
       <c r="W22" t="n">
-        <v>0.1010873064337002</v>
+        <v>2.536917975280589</v>
       </c>
       <c r="X22" t="n">
-        <v>0.06582499622624763</v>
+        <v>3.393729214158444</v>
       </c>
       <c r="Y22" t="n">
-        <v>0.1856678216841803</v>
+        <v>3.628694629825319</v>
       </c>
       <c r="Z22" t="n">
-        <v>0.01797030155824769</v>
+        <v>1.096673806588542</v>
       </c>
       <c r="AA22" t="n">
-        <v>0.06228426876297948</v>
+        <v>2.234166020025718</v>
       </c>
       <c r="AB22" t="n">
-        <v>0.07728369754581042</v>
+        <v>1.765035193625475</v>
       </c>
       <c r="AC22" t="n">
-        <v>0.07892968564032693</v>
+        <v>3.355253747923689</v>
       </c>
       <c r="AD22" t="n">
-        <v>0.07383131754107036</v>
+        <v>2.782647696923506</v>
       </c>
       <c r="AE22" t="n">
-        <v>0.2171427603954774</v>
+        <v>4.283221414798501</v>
       </c>
     </row>
     <row r="23">
@@ -2525,94 +2525,94 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>0.1899452753901378</v>
+        <v>6.360367957504774</v>
       </c>
       <c r="C23" t="n">
-        <v>0.04223690453943452</v>
+        <v>2.349546033947658</v>
       </c>
       <c r="D23" t="n">
-        <v>0.1204142087585774</v>
+        <v>2.486013600115259</v>
       </c>
       <c r="E23" t="n">
-        <v>0.09973867328811044</v>
+        <v>3.900903113150885</v>
       </c>
       <c r="F23" t="n">
-        <v>0.1164697180672883</v>
+        <v>3.496330651214064</v>
       </c>
       <c r="G23" t="n">
-        <v>0.05070744053651875</v>
+        <v>2.926584250984807</v>
       </c>
       <c r="H23" t="n">
-        <v>0.06831350358760413</v>
+        <v>4.102141763659696</v>
       </c>
       <c r="I23" t="n">
-        <v>0.1034215468999604</v>
+        <v>2.757108656951327</v>
       </c>
       <c r="J23" t="n">
-        <v>0.1037425367117263</v>
+        <v>2.584453310344512</v>
       </c>
       <c r="K23" t="n">
-        <v>0.0435723321353472</v>
+        <v>2.767004934487564</v>
       </c>
       <c r="L23" t="n">
-        <v>0.06586915371418693</v>
+        <v>2.251554274048607</v>
       </c>
       <c r="M23" t="n">
-        <v>0.06949785456299067</v>
+        <v>2.254483704351522</v>
       </c>
       <c r="N23" t="n">
-        <v>0.1463375744119478</v>
+        <v>2.536755405230279</v>
       </c>
       <c r="O23" t="n">
-        <v>0.0632800353510565</v>
+        <v>2.507313357982912</v>
       </c>
       <c r="P23" t="n">
-        <v>0.09829631881750918</v>
+        <v>2.975092834828807</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.2072033993866904</v>
+        <v>4.987206341788692</v>
       </c>
       <c r="R23" t="n">
-        <v>0.1642773486842691</v>
+        <v>4.66810129394759</v>
       </c>
       <c r="S23" t="n">
-        <v>0.1587973020634575</v>
+        <v>4.26411015053906</v>
       </c>
       <c r="T23" t="n">
-        <v>0.03502579071543321</v>
+        <v>2.737587857702662</v>
       </c>
       <c r="U23" t="n">
-        <v>0.2160186059144839</v>
+        <v>4.992074112235162</v>
       </c>
       <c r="V23" t="n">
-        <v>0.1010873064337002</v>
+        <v>2.536917975280589</v>
       </c>
       <c r="W23" t="n">
         <v>0</v>
       </c>
       <c r="X23" t="n">
-        <v>0.1294789501064717</v>
+        <v>5.416806887472846</v>
       </c>
       <c r="Y23" t="n">
-        <v>0.0976780717563821</v>
+        <v>3.169558015225392</v>
       </c>
       <c r="Z23" t="n">
-        <v>0.09926238207436316</v>
+        <v>3.229665432496514</v>
       </c>
       <c r="AA23" t="n">
-        <v>0.1570565153086543</v>
+        <v>4.573364492644952</v>
       </c>
       <c r="AB23" t="n">
-        <v>0.06313120907300399</v>
+        <v>3.05496309006026</v>
       </c>
       <c r="AC23" t="n">
-        <v>0.1722036949311583</v>
+        <v>5.670693986484338</v>
       </c>
       <c r="AD23" t="n">
-        <v>0.1665512377378904</v>
+        <v>5.068327599469267</v>
       </c>
       <c r="AE23" t="n">
-        <v>0.1233163600273979</v>
+        <v>3.084024283366406</v>
       </c>
     </row>
     <row r="24">
@@ -2620,94 +2620,94 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>0.06581907329878174</v>
+        <v>1.637300194075228</v>
       </c>
       <c r="C24" t="n">
-        <v>0.111020922625073</v>
+        <v>3.341477486609099</v>
       </c>
       <c r="D24" t="n">
-        <v>0.07563297178059294</v>
+        <v>4.808886555729749</v>
       </c>
       <c r="E24" t="n">
-        <v>0.04984292570229198</v>
+        <v>2.955490887209062</v>
       </c>
       <c r="F24" t="n">
-        <v>0.03385478775342152</v>
+        <v>2.324685075560781</v>
       </c>
       <c r="G24" t="n">
-        <v>0.09255668912323532</v>
+        <v>3.346802053074101</v>
       </c>
       <c r="H24" t="n">
-        <v>0.1069737984950122</v>
+        <v>2.061539444301041</v>
       </c>
       <c r="I24" t="n">
-        <v>0.08311847075483152</v>
+        <v>4.747899255812637</v>
       </c>
       <c r="J24" t="n">
-        <v>0.2136556111732859</v>
+        <v>7.307375887821482</v>
       </c>
       <c r="K24" t="n">
-        <v>0.09587401102562401</v>
+        <v>3.758482226017929</v>
       </c>
       <c r="L24" t="n">
-        <v>0.1591848790030104</v>
+        <v>4.222584733571623</v>
       </c>
       <c r="M24" t="n">
-        <v>0.1635362526013421</v>
+        <v>4.725646503799299</v>
       </c>
       <c r="N24" t="n">
-        <v>0.1189611972094547</v>
+        <v>5.877434064007069</v>
       </c>
       <c r="O24" t="n">
-        <v>0.1433053590036265</v>
+        <v>3.848829194791297</v>
       </c>
       <c r="P24" t="n">
-        <v>0.05194549270057697</v>
+        <v>2.731135044305354</v>
       </c>
       <c r="Q24" t="n">
-        <v>0.1093968924166139</v>
+        <v>2.188515595787691</v>
       </c>
       <c r="R24" t="n">
-        <v>0.05957146884096129</v>
+        <v>1.601082265043603</v>
       </c>
       <c r="S24" t="n">
-        <v>0.08300995717850779</v>
+        <v>3.282453765497387</v>
       </c>
       <c r="T24" t="n">
-        <v>0.1053349215250191</v>
+        <v>3.243077592389029</v>
       </c>
       <c r="U24" t="n">
-        <v>0.1249036799493486</v>
+        <v>2.761215662975023</v>
       </c>
       <c r="V24" t="n">
-        <v>0.06582499622624763</v>
+        <v>3.393729214158444</v>
       </c>
       <c r="W24" t="n">
-        <v>0.1294789501064717</v>
+        <v>5.416806887472846</v>
       </c>
       <c r="X24" t="n">
         <v>0</v>
       </c>
       <c r="Y24" t="n">
-        <v>0.1853409759910433</v>
+        <v>4.413095423444767</v>
       </c>
       <c r="Z24" t="n">
-        <v>0.05488087927823531</v>
+        <v>2.754863914414496</v>
       </c>
       <c r="AA24" t="n">
-        <v>0.05264424173495154</v>
+        <v>1.493849550471355</v>
       </c>
       <c r="AB24" t="n">
-        <v>0.07332924353967864</v>
+        <v>2.514489232628591</v>
       </c>
       <c r="AC24" t="n">
-        <v>0.05885276747926563</v>
+        <v>1.063103421771199</v>
       </c>
       <c r="AD24" t="n">
-        <v>0.05416599535860364</v>
+        <v>1.116812604446021</v>
       </c>
       <c r="AE24" t="n">
-        <v>0.2197321716126216</v>
+        <v>5.314309904690702</v>
       </c>
     </row>
     <row r="25">
@@ -2715,94 +2715,94 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>0.2459834353226894</v>
+        <v>5.712427156349889</v>
       </c>
       <c r="C25" t="n">
-        <v>0.08213880702039783</v>
+        <v>2.240793072687274</v>
       </c>
       <c r="D25" t="n">
-        <v>0.2063163315849977</v>
+        <v>4.054397494436631</v>
       </c>
       <c r="E25" t="n">
-        <v>0.1680626542925896</v>
+        <v>4.403301790244883</v>
       </c>
       <c r="F25" t="n">
-        <v>0.1867814204719543</v>
+        <v>3.797037030146567</v>
       </c>
       <c r="G25" t="n">
-        <v>0.1067694135644514</v>
+        <v>3.305921909914511</v>
       </c>
       <c r="H25" t="n">
-        <v>0.07865944609262772</v>
+        <v>2.435435208114233</v>
       </c>
       <c r="I25" t="n">
-        <v>0.1917395403190078</v>
+        <v>4.863815223135096</v>
       </c>
       <c r="J25" t="n">
-        <v>0.04758213546145978</v>
+        <v>3.863885889324671</v>
       </c>
       <c r="K25" t="n">
-        <v>0.1126023542305641</v>
+        <v>3.639812296398546</v>
       </c>
       <c r="L25" t="n">
-        <v>0.03247173365975001</v>
+        <v>1.008200803432199</v>
       </c>
       <c r="M25" t="n">
-        <v>0.02837070400902465</v>
+        <v>1.014751470146016</v>
       </c>
       <c r="N25" t="n">
-        <v>0.2397047406442568</v>
+        <v>5.177568356281527</v>
       </c>
       <c r="O25" t="n">
-        <v>0.048146010899878</v>
+        <v>1.913281079604493</v>
       </c>
       <c r="P25" t="n">
-        <v>0.1774060249428374</v>
+        <v>3.596335204532062</v>
       </c>
       <c r="Q25" t="n">
-        <v>0.2850144760492523</v>
+        <v>5.178911449765597</v>
       </c>
       <c r="R25" t="n">
-        <v>0.2364994698977393</v>
+        <v>4.449983453728541</v>
       </c>
       <c r="S25" t="n">
-        <v>0.2408986538741369</v>
+        <v>5.292281537201471</v>
       </c>
       <c r="T25" t="n">
-        <v>0.09880706708484376</v>
+        <v>2.09242044539375</v>
       </c>
       <c r="U25" t="n">
-        <v>0.2972676261132158</v>
+        <v>5.669229892955243</v>
       </c>
       <c r="V25" t="n">
-        <v>0.1856678216841803</v>
+        <v>3.628694629825319</v>
       </c>
       <c r="W25" t="n">
-        <v>0.0976780717563821</v>
+        <v>3.169558015225392</v>
       </c>
       <c r="X25" t="n">
-        <v>0.1853409759910433</v>
+        <v>4.413095423444767</v>
       </c>
       <c r="Y25" t="n">
         <v>0</v>
       </c>
       <c r="Z25" t="n">
-        <v>0.1778021902221092</v>
+        <v>3.35655937202182</v>
       </c>
       <c r="AA25" t="n">
-        <v>0.2291274706281275</v>
+        <v>4.47875482117738</v>
       </c>
       <c r="AB25" t="n">
-        <v>0.1153266688433786</v>
+        <v>2.361788937564758</v>
       </c>
       <c r="AC25" t="n">
-        <v>0.2401109905279437</v>
+        <v>5.00659137486737</v>
       </c>
       <c r="AD25" t="n">
-        <v>0.235487653099966</v>
+        <v>4.748416315463147</v>
       </c>
       <c r="AE25" t="n">
-        <v>0.04095623385809211</v>
+        <v>2.438652128120081</v>
       </c>
     </row>
     <row r="26">
@@ -2810,94 +2810,94 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>0.106795820175408</v>
+        <v>3.988916103650405</v>
       </c>
       <c r="C26" t="n">
-        <v>0.09982106388597427</v>
+        <v>2.227514640590237</v>
       </c>
       <c r="D26" t="n">
-        <v>0.03299209730288376</v>
+        <v>2.112175570209989</v>
       </c>
       <c r="E26" t="n">
-        <v>0.05157416996268419</v>
+        <v>3.027866510911047</v>
       </c>
       <c r="F26" t="n">
-        <v>0.03870268494845793</v>
+        <v>1.680075056941001</v>
       </c>
       <c r="G26" t="n">
-        <v>0.0829667021737379</v>
+        <v>2.815801482028545</v>
       </c>
       <c r="H26" t="n">
-        <v>0.1076169449191333</v>
+        <v>2.46955197292034</v>
       </c>
       <c r="I26" t="n">
-        <v>0.04880611180630125</v>
+        <v>3.38445080783804</v>
       </c>
       <c r="J26" t="n">
-        <v>0.1981674589814975</v>
+        <v>5.555508771377668</v>
       </c>
       <c r="K26" t="n">
-        <v>0.07913716203808327</v>
+        <v>3.032039790480433</v>
       </c>
       <c r="L26" t="n">
-        <v>0.1475424493702578</v>
+        <v>2.820034553832355</v>
       </c>
       <c r="M26" t="n">
-        <v>0.1516576549637516</v>
+        <v>3.086620502949681</v>
       </c>
       <c r="N26" t="n">
-        <v>0.07676070911372927</v>
+        <v>3.364356727353928</v>
       </c>
       <c r="O26" t="n">
-        <v>0.1363391253771885</v>
+        <v>2.974758535670767</v>
       </c>
       <c r="P26" t="n">
-        <v>0.01842342542976349</v>
+        <v>1.215086795697153</v>
       </c>
       <c r="Q26" t="n">
-        <v>0.1100084656472157</v>
+        <v>2.099837069023817</v>
       </c>
       <c r="R26" t="n">
-        <v>0.06684733808302573</v>
+        <v>1.647103031328638</v>
       </c>
       <c r="S26" t="n">
-        <v>0.07325439192003551</v>
+        <v>3.052157723170735</v>
       </c>
       <c r="T26" t="n">
-        <v>0.08155459011418004</v>
+        <v>1.368953100373821</v>
       </c>
       <c r="U26" t="n">
-        <v>0.1226115853716651</v>
+        <v>2.813572345407069</v>
       </c>
       <c r="V26" t="n">
-        <v>0.01797030155824769</v>
+        <v>1.096673806588542</v>
       </c>
       <c r="W26" t="n">
-        <v>0.09926238207436316</v>
+        <v>3.229665432496514</v>
       </c>
       <c r="X26" t="n">
-        <v>0.05488087927823531</v>
+        <v>2.754863914414496</v>
       </c>
       <c r="Y26" t="n">
-        <v>0.1778021902221092</v>
+        <v>3.35655937202182</v>
       </c>
       <c r="Z26" t="n">
         <v>0</v>
       </c>
       <c r="AA26" t="n">
-        <v>0.06202371238193756</v>
+        <v>1.880321411709889</v>
       </c>
       <c r="AB26" t="n">
-        <v>0.06782427227882014</v>
+        <v>1.397185684535516</v>
       </c>
       <c r="AC26" t="n">
-        <v>0.07531759989795615</v>
+        <v>2.653138319784209</v>
       </c>
       <c r="AD26" t="n">
-        <v>0.07233892151346578</v>
+        <v>2.364593768758778</v>
       </c>
       <c r="AE26" t="n">
-        <v>0.2113111997245407</v>
+        <v>4.55633628270397</v>
       </c>
     </row>
     <row r="27">
@@ -2905,94 +2905,94 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>0.05554315646779839</v>
+        <v>2.21124761847412</v>
       </c>
       <c r="C27" t="n">
-        <v>0.1499077543743874</v>
+        <v>2.899974565947792</v>
       </c>
       <c r="D27" t="n">
-        <v>0.05621275750246625</v>
+        <v>3.691168026956802</v>
       </c>
       <c r="E27" t="n">
-        <v>0.07164419693174851</v>
+        <v>2.256805260881249</v>
       </c>
       <c r="F27" t="n">
-        <v>0.04534498745110666</v>
+        <v>1.271772742695402</v>
       </c>
       <c r="G27" t="n">
-        <v>0.1287128126576745</v>
+        <v>2.813991408063055</v>
       </c>
       <c r="H27" t="n">
-        <v>0.152668281102907</v>
+        <v>2.538761578120648</v>
       </c>
       <c r="I27" t="n">
-        <v>0.07456423046973475</v>
+        <v>3.581523944900341</v>
       </c>
       <c r="J27" t="n">
-        <v>0.2519989740757531</v>
+        <v>6.751193815342231</v>
       </c>
       <c r="K27" t="n">
-        <v>0.1272818106757521</v>
+        <v>3.084375166557323</v>
       </c>
       <c r="L27" t="n">
-        <v>0.2002507290216913</v>
+        <v>3.994630997121353</v>
       </c>
       <c r="M27" t="n">
-        <v>0.2047260776834877</v>
+        <v>4.460909353845585</v>
       </c>
       <c r="N27" t="n">
-        <v>0.08625198607646963</v>
+        <v>4.578672254166672</v>
       </c>
       <c r="O27" t="n">
-        <v>0.1853172733942032</v>
+        <v>3.609283516669732</v>
       </c>
       <c r="P27" t="n">
-        <v>0.05919456782280713</v>
+        <v>1.617213135699892</v>
       </c>
       <c r="Q27" t="n">
-        <v>0.058512015827461</v>
+        <v>1.014508839393335</v>
       </c>
       <c r="R27" t="n">
-        <v>0.01202558997330699</v>
+        <v>0.6506224729803936</v>
       </c>
       <c r="S27" t="n">
-        <v>0.0399551997674322</v>
+        <v>2.13799710751497</v>
       </c>
       <c r="T27" t="n">
-        <v>0.1391026047535804</v>
+        <v>2.86672296401834</v>
       </c>
       <c r="U27" t="n">
-        <v>0.07256016988428485</v>
+        <v>1.503997662167468</v>
       </c>
       <c r="V27" t="n">
-        <v>0.06228426876297948</v>
+        <v>2.234166020025718</v>
       </c>
       <c r="W27" t="n">
-        <v>0.1570565153086543</v>
+        <v>4.573364492644952</v>
       </c>
       <c r="X27" t="n">
-        <v>0.05264424173495154</v>
+        <v>1.493849550471355</v>
       </c>
       <c r="Y27" t="n">
-        <v>0.2291274706281275</v>
+        <v>4.47875482117738</v>
       </c>
       <c r="Z27" t="n">
-        <v>0.06202371238193756</v>
+        <v>1.880321411709889</v>
       </c>
       <c r="AA27" t="n">
         <v>0</v>
       </c>
       <c r="AB27" t="n">
-        <v>0.1139468733880041</v>
+        <v>2.156183211855545</v>
       </c>
       <c r="AC27" t="n">
-        <v>0.02207344202597201</v>
+        <v>1.352514716627487</v>
       </c>
       <c r="AD27" t="n">
-        <v>0.01219548671597912</v>
+        <v>0.5603103379461772</v>
       </c>
       <c r="AE27" t="n">
-        <v>0.2622071312343647</v>
+        <v>5.214457775711872</v>
       </c>
     </row>
     <row r="28">
@@ -3000,94 +3000,94 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>0.1357325824031616</v>
+        <v>3.735023094091162</v>
       </c>
       <c r="C28" t="n">
-        <v>0.03824743763421085</v>
+        <v>1.18661481226105</v>
       </c>
       <c r="D28" t="n">
-        <v>0.09829304000566533</v>
+        <v>2.932309990850223</v>
       </c>
       <c r="E28" t="n">
-        <v>0.05768569364452938</v>
+        <v>2.543253394995025</v>
       </c>
       <c r="F28" t="n">
-        <v>0.07191582730154523</v>
+        <v>1.523582850402275</v>
       </c>
       <c r="G28" t="n">
-        <v>0.02733068502701801</v>
+        <v>1.966937345663825</v>
       </c>
       <c r="H28" t="n">
-        <v>0.0409977708487627</v>
+        <v>1.344213039559745</v>
       </c>
       <c r="I28" t="n">
-        <v>0.08825400647815823</v>
+        <v>3.386952358182625</v>
       </c>
       <c r="J28" t="n">
-        <v>0.1407763291467648</v>
+        <v>4.921716305777493</v>
       </c>
       <c r="K28" t="n">
-        <v>0.03447766186165483</v>
+        <v>2.366146447410879</v>
       </c>
       <c r="L28" t="n">
-        <v>0.08693046847478607</v>
+        <v>1.878451524076348</v>
       </c>
       <c r="M28" t="n">
-        <v>0.09141891301050482</v>
+        <v>2.335110092897443</v>
       </c>
       <c r="N28" t="n">
-        <v>0.138573059310039</v>
+        <v>4.089424653742001</v>
       </c>
       <c r="O28" t="n">
-        <v>0.07221681081132462</v>
+        <v>1.78930682713557</v>
       </c>
       <c r="P28" t="n">
-        <v>0.06523550110603832</v>
+        <v>1.4247580709917</v>
       </c>
       <c r="Q28" t="n">
-        <v>0.1704743870869087</v>
+        <v>2.88156214656459</v>
       </c>
       <c r="R28" t="n">
-        <v>0.1217163835627062</v>
+        <v>2.193384957508877</v>
       </c>
       <c r="S28" t="n">
-        <v>0.1280817178360158</v>
+        <v>3.172784562222847</v>
       </c>
       <c r="T28" t="n">
-        <v>0.03929662516899492</v>
+        <v>1.153107146047482</v>
       </c>
       <c r="U28" t="n">
-        <v>0.1828658026562699</v>
+        <v>3.342572875309702</v>
       </c>
       <c r="V28" t="n">
-        <v>0.07728369754581042</v>
+        <v>1.765035193625475</v>
       </c>
       <c r="W28" t="n">
-        <v>0.06313120907300399</v>
+        <v>3.05496309006026</v>
       </c>
       <c r="X28" t="n">
-        <v>0.07332924353967864</v>
+        <v>2.514489232628591</v>
       </c>
       <c r="Y28" t="n">
-        <v>0.1153266688433786</v>
+        <v>2.361788937564758</v>
       </c>
       <c r="Z28" t="n">
-        <v>0.06782427227882014</v>
+        <v>1.397185684535516</v>
       </c>
       <c r="AA28" t="n">
-        <v>0.1139468733880041</v>
+        <v>2.156183211855545</v>
       </c>
       <c r="AB28" t="n">
         <v>0</v>
       </c>
       <c r="AC28" t="n">
-        <v>0.126026357411171</v>
+        <v>2.945669927987106</v>
       </c>
       <c r="AD28" t="n">
-        <v>0.120554575084416</v>
+        <v>2.500375670680219</v>
       </c>
       <c r="AE28" t="n">
-        <v>0.1489642910297401</v>
+        <v>3.414262855430317</v>
       </c>
     </row>
     <row r="29">
@@ -3095,94 +3095,94 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>0.05226604243798294</v>
+        <v>2.013613563952808</v>
       </c>
       <c r="C29" t="n">
-        <v>0.1633172698707854</v>
+        <v>3.884251233197155</v>
       </c>
       <c r="D29" t="n">
-        <v>0.07127289197002133</v>
+        <v>4.620856073568758</v>
       </c>
       <c r="E29" t="n">
-        <v>0.08950514403305625</v>
+        <v>3.417338753062894</v>
       </c>
       <c r="F29" t="n">
-        <v>0.06263733342079285</v>
+        <v>2.557353822897833</v>
       </c>
       <c r="G29" t="n">
-        <v>0.1436581071823157</v>
+        <v>3.933073178588527</v>
       </c>
       <c r="H29" t="n">
-        <v>0.1630230937439195</v>
+        <v>2.862122730740311</v>
       </c>
       <c r="I29" t="n">
-        <v>0.09537928954806282</v>
+        <v>4.908668844500274</v>
       </c>
       <c r="J29" t="n">
-        <v>0.2658353880051486</v>
+        <v>7.801804017879788</v>
       </c>
       <c r="K29" t="n">
-        <v>0.1433635878474069</v>
+        <v>4.267499655479162</v>
       </c>
       <c r="L29" t="n">
-        <v>0.2123699603631284</v>
+        <v>4.754534625479854</v>
       </c>
       <c r="M29" t="n">
-        <v>0.2166223082488395</v>
+        <v>5.187096518951847</v>
       </c>
       <c r="N29" t="n">
-        <v>0.09984792019169891</v>
+        <v>5.685022832115944</v>
       </c>
       <c r="O29" t="n">
-        <v>0.1979948880899807</v>
+        <v>4.515381444009831</v>
       </c>
       <c r="P29" t="n">
-        <v>0.07630925066796164</v>
+        <v>2.835949959353229</v>
       </c>
       <c r="Q29" t="n">
-        <v>0.05291877158688211</v>
+        <v>1.49367187264913</v>
       </c>
       <c r="R29" t="n">
-        <v>0.01441431731969894</v>
+        <v>1.165778089047655</v>
       </c>
       <c r="S29" t="n">
-        <v>0.05821637843368258</v>
+        <v>3.33475331197733</v>
       </c>
       <c r="T29" t="n">
-        <v>0.1511139983226706</v>
+        <v>3.482268086760989</v>
       </c>
       <c r="U29" t="n">
-        <v>0.07246672653759842</v>
+        <v>2.392409977351756</v>
       </c>
       <c r="V29" t="n">
-        <v>0.07892968564032693</v>
+        <v>3.355253747923689</v>
       </c>
       <c r="W29" t="n">
-        <v>0.1722036949311583</v>
+        <v>5.670693986484338</v>
       </c>
       <c r="X29" t="n">
-        <v>0.05885276747926563</v>
+        <v>1.063103421771199</v>
       </c>
       <c r="Y29" t="n">
-        <v>0.2401109905279437</v>
+        <v>5.00659137486737</v>
       </c>
       <c r="Z29" t="n">
-        <v>0.07531759989795615</v>
+        <v>2.653138319784209</v>
       </c>
       <c r="AA29" t="n">
-        <v>0.02207344202597201</v>
+        <v>1.352514716627487</v>
       </c>
       <c r="AB29" t="n">
-        <v>0.126026357411171</v>
+        <v>2.945669927987106</v>
       </c>
       <c r="AC29" t="n">
         <v>0</v>
       </c>
       <c r="AD29" t="n">
-        <v>0.01612870453015248</v>
+        <v>1.013229379767134</v>
       </c>
       <c r="AE29" t="n">
-        <v>0.2747643075050763</v>
+        <v>6.071030736944571</v>
       </c>
     </row>
     <row r="30">
@@ -3190,94 +3190,94 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>0.04506818649620872</v>
+        <v>1.701564685390132</v>
       </c>
       <c r="C30" t="n">
-        <v>0.157114999240016</v>
+        <v>3.252804243130963</v>
       </c>
       <c r="D30" t="n">
-        <v>0.06827564202121632</v>
+        <v>4.237882719954387</v>
       </c>
       <c r="E30" t="n">
-        <v>0.07846509541308951</v>
+        <v>2.449897008075816</v>
       </c>
       <c r="F30" t="n">
-        <v>0.05283696998456832</v>
+        <v>1.70533920383869</v>
       </c>
       <c r="G30" t="n">
-        <v>0.1359434080425483</v>
+        <v>3.10136358871117</v>
       </c>
       <c r="H30" t="n">
-        <v>0.1581338667132727</v>
+        <v>2.608674232462378</v>
       </c>
       <c r="I30" t="n">
-        <v>0.08567135848253715</v>
+        <v>4.014706852493398</v>
       </c>
       <c r="J30" t="n">
-        <v>0.2597030811356905</v>
+        <v>7.173335204743243</v>
       </c>
       <c r="K30" t="n">
-        <v>0.1354004383445294</v>
+        <v>3.404176755905457</v>
       </c>
       <c r="L30" t="n">
-        <v>0.2072976474389855</v>
+        <v>4.339606747773769</v>
       </c>
       <c r="M30" t="n">
-        <v>0.2117784626108641</v>
+        <v>4.830246499010525</v>
       </c>
       <c r="N30" t="n">
-        <v>0.09726082461286675</v>
+        <v>5.134173783153908</v>
       </c>
       <c r="O30" t="n">
-        <v>0.1918565697619008</v>
+        <v>3.906025157657836</v>
       </c>
       <c r="P30" t="n">
-        <v>0.06949132193266785</v>
+        <v>2.131754661178397</v>
       </c>
       <c r="Q30" t="n">
-        <v>0.05672623030059108</v>
+        <v>1.239298588369926</v>
       </c>
       <c r="R30" t="n">
-        <v>0.01495660068341693</v>
+        <v>0.9286345308215204</v>
       </c>
       <c r="S30" t="n">
-        <v>0.04766195734996809</v>
+        <v>2.394412596012076</v>
       </c>
       <c r="T30" t="n">
-        <v>0.1474567957062103</v>
+        <v>3.251018594262992</v>
       </c>
       <c r="U30" t="n">
-        <v>0.07184335996326389</v>
+        <v>1.678718479843614</v>
       </c>
       <c r="V30" t="n">
-        <v>0.07383131754107036</v>
+        <v>2.782647696923506</v>
       </c>
       <c r="W30" t="n">
-        <v>0.1665512377378904</v>
+        <v>5.068327599469267</v>
       </c>
       <c r="X30" t="n">
-        <v>0.05416599535860364</v>
+        <v>1.116812604446021</v>
       </c>
       <c r="Y30" t="n">
-        <v>0.235487653099966</v>
+        <v>4.748416315463147</v>
       </c>
       <c r="Z30" t="n">
-        <v>0.07233892151346578</v>
+        <v>2.364593768758778</v>
       </c>
       <c r="AA30" t="n">
-        <v>0.01219548671597912</v>
+        <v>0.5603103379461772</v>
       </c>
       <c r="AB30" t="n">
-        <v>0.120554575084416</v>
+        <v>2.500375670680219</v>
       </c>
       <c r="AC30" t="n">
-        <v>0.01612870453015248</v>
+        <v>1.013229379767134</v>
       </c>
       <c r="AD30" t="n">
         <v>0</v>
       </c>
       <c r="AE30" t="n">
-        <v>0.2688083955976159</v>
+        <v>5.473608282277119</v>
       </c>
     </row>
     <row r="31">
@@ -3285,91 +3285,91 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>0.2780711605469107</v>
+        <v>6.091820854177365</v>
       </c>
       <c r="C31" t="n">
-        <v>0.1127749837285775</v>
+        <v>2.419703202153505</v>
       </c>
       <c r="D31" t="n">
-        <v>0.238154108792853</v>
+        <v>5.034943134914101</v>
       </c>
       <c r="E31" t="n">
-        <v>0.1970189886359818</v>
+        <v>3.982842182560028</v>
       </c>
       <c r="F31" t="n">
-        <v>0.2183983569917965</v>
+        <v>4.184849121853958</v>
       </c>
       <c r="G31" t="n">
-        <v>0.135194783972139</v>
+        <v>2.750610897135713</v>
       </c>
       <c r="H31" t="n">
-        <v>0.1137997480336771</v>
+        <v>3.461875241184558</v>
       </c>
       <c r="I31" t="n">
-        <v>0.2187423493498997</v>
+        <v>4.22249184824608</v>
       </c>
       <c r="J31" t="n">
-        <v>0.03095435531326302</v>
+        <v>2.787482330431697</v>
       </c>
       <c r="K31" t="n">
-        <v>0.1396224029375165</v>
+        <v>2.867477162477153</v>
       </c>
       <c r="L31" t="n">
-        <v>0.06471658377099473</v>
+        <v>2.097788228018719</v>
       </c>
       <c r="M31" t="n">
-        <v>0.06159353181354079</v>
+        <v>2.459343166866641</v>
       </c>
       <c r="N31" t="n">
-        <v>0.2686522967267873</v>
+        <v>5.481667918899217</v>
       </c>
       <c r="O31" t="n">
-        <v>0.07704689741252965</v>
+        <v>1.664699071974984</v>
       </c>
       <c r="P31" t="n">
-        <v>0.2090424202941703</v>
+        <v>4.102973629951916</v>
       </c>
       <c r="Q31" t="n">
-        <v>0.3182655032197653</v>
+        <v>6.061348784835237</v>
       </c>
       <c r="R31" t="n">
-        <v>0.2703665663826597</v>
+        <v>5.475393427086924</v>
       </c>
       <c r="S31" t="n">
-        <v>0.2704513459680312</v>
+        <v>5.088489688151256</v>
       </c>
       <c r="T31" t="n">
-        <v>0.1327338608457503</v>
+        <v>3.595147026549128</v>
       </c>
       <c r="U31" t="n">
-        <v>0.3287483354548894</v>
+        <v>6.007126894520279</v>
       </c>
       <c r="V31" t="n">
-        <v>0.2171427603954774</v>
+        <v>4.283221414798501</v>
       </c>
       <c r="W31" t="n">
-        <v>0.1233163600273979</v>
+        <v>3.084024283366406</v>
       </c>
       <c r="X31" t="n">
-        <v>0.2197321716126216</v>
+        <v>5.314309904690702</v>
       </c>
       <c r="Y31" t="n">
-        <v>0.04095623385809211</v>
+        <v>2.438652128120081</v>
       </c>
       <c r="Z31" t="n">
-        <v>0.2113111997245407</v>
+        <v>4.55633628270397</v>
       </c>
       <c r="AA31" t="n">
-        <v>0.2622071312343647</v>
+        <v>5.214457775711872</v>
       </c>
       <c r="AB31" t="n">
-        <v>0.1489642910297401</v>
+        <v>3.414262855430317</v>
       </c>
       <c r="AC31" t="n">
-        <v>0.2747643075050763</v>
+        <v>6.071030736944571</v>
       </c>
       <c r="AD31" t="n">
-        <v>0.2688083955976159</v>
+        <v>5.473608282277119</v>
       </c>
       <c r="AE31" t="n">
         <v>0</v>

</xml_diff>